<commit_message>
Merged PR 1305: Release-doc generation script and template updates
PS Script:
- Added error check for MS-Word spell tags that corrupt placeholder vars.
- Added var substitution for contents of var-input file so as long as another var is defined above it, a var can use that var inside its value.
- Get env and release ID values from input file now.
- Create local temp folder to house the generated rel doc.
- Output URL to file uploaded to web server.
Other:
- To HTM template: added placeholders to support: special release branch info, task after IRMA DB update, manual mammoth deploy.
- Prod values for input sheet.
- Removing QA doc I'd checked in.

Related work items: #29937
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
     <sheet name="Prod" sheetId="2" r:id="rId2"/>
+    <sheet name="other ideas" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -25,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="140">
   <si>
     <t>Key</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>Template</t>
   </si>
   <si>
@@ -189,12 +187,6 @@
     <t>IconBuildId</t>
   </si>
   <si>
-    <t>PropFilesListSection</t>
-  </si>
-  <si>
-    <t>TIBCO section listing deployable artifact links (.properties files)</t>
-  </si>
-  <si>
     <t>IconReleaseBranchName</t>
   </si>
   <si>
@@ -235,9 +227,6 @@
   </si>
   <si>
     <t>.</t>
-  </si>
-  <si>
-    <t>comingsoon</t>
   </si>
   <si>
     <t>FullDbList</t>
@@ -356,10 +345,110 @@
     <t>*NONE*</t>
   </si>
   <si>
-    <t>Prd</t>
-  </si>
-  <si>
     <t>coming_soon</t>
+  </si>
+  <si>
+    <t>AdditionalIrmaComponentDeploySection</t>
+  </si>
+  <si>
+    <t>Usually a link to a component-deploy script, such as "IRMA Release Launcher" powershell</t>
+  </si>
+  <si>
+    <t>Open folder &lt;a href="\\irmaqafile\e$\irma\Staging\Release\Launcher"&gt;Release Launcher Folder&lt;/a&gt;.  Right-click script "IRMA Release Launcher.__IrmaReleaseLauncherVersionRef__.%env%.ps1" &gt; Run with PowerShell…</t>
+  </si>
+  <si>
+    <t>IrmaReleaseLauncherVersionRef</t>
+  </si>
+  <si>
+    <t>Value (NOTE: cannot contain new-line chars)</t>
+  </si>
+  <si>
+    <t>ReleaseYear</t>
+  </si>
+  <si>
+    <t>ReleaseId</t>
+  </si>
+  <si>
+    <t>PRD</t>
+  </si>
+  <si>
+    <t>Mammoth-DB01-Prd\Mammoth</t>
+  </si>
+  <si>
+    <t>IDP-Icon\Shared3P</t>
+  </si>
+  <si>
+    <t>IDP-xx\xxP</t>
+  </si>
+  <si>
+    <t>IRMAPrdApp[1-8]</t>
+  </si>
+  <si>
+    <t>Mammoth-App01-QA, IRMAPrdApp[9-10]</t>
+  </si>
+  <si>
+    <t>VM-Icon-Prd[1-6]</t>
+  </si>
+  <si>
+    <t>SpecialIconReleaseDetails</t>
+  </si>
+  <si>
+    <t>SpecialIrmaReleaseDetails</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;</t>
+  </si>
+  <si>
+    <t>After main Mammoth VSTS release, run release: 'RELEASE_FastTrack_Sprints127-128' branch, deploy: Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>AdditionalIrmaDeployImplementerRef</t>
+  </si>
+  <si>
+    <t>SysMgmt, Apps/Tools</t>
+  </si>
+  <si>
+    <t>AdditionalIrmaComponentList</t>
+  </si>
+  <si>
+    <t>Open folder &lt;a href="\\irmaqafile\e$\irma\Staging\Release\Launcher"&gt;Release Launcher Folder&lt;/a&gt;.  Right-click script "IRMA Release Launcher.__IrmaReleaseLauncherVersionRef__.__TargetEnvShort__.ps1" &gt; Run with PowerShell&lt;br&gt;__AdditionalIrmaComponentList__</t>
+  </si>
+  <si>
+    <t>**Components**: IRMA Mobile Plugin (FL-Region Only), WFMUHS</t>
+  </si>
+  <si>
+    <t>MammothActivePriceService</t>
+  </si>
+  <si>
+    <t>QA: CERD1673, CERD1674 | QA-Perf: CERD1662, CERD1663, CERD1664, CERD1665
+Prod: cerp1643, cerp1644, odrp1634, odrp1635</t>
+  </si>
+  <si>
+    <t>Prod: cerp1643, cerp1644, odrp1634, odrp1635</t>
+  </si>
+  <si>
+    <t>IrmaPostDbUpdateTask</t>
+  </si>
+  <si>
+    <t>Special Task</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;Additional special-fixes build, 'RELEASE_FastTrack_Sprints127-128' branch, build=20181030.1</t>
+  </si>
+  <si>
+    <t>&lt;a href="file://irmaqafile/e$/IRMA/Staging/iCon/__IconVer__/DB/Icon%20__IconVer__%20Updates.sql"&gt;Icon __IconVer__ DB Updates&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>&lt;span style='background:lime;mso-highlight:lime'&gt;**Start Price-Batch Purge ASAP** (see separate doc)&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>None, continue</t>
+  </si>
+  <si>
+    <t>CHG0033369</t>
   </si>
 </sst>
 </file>
@@ -378,12 +467,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -398,10 +493,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -718,16 +820,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C44" sqref="A2:C44"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="42.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
@@ -739,76 +841,76 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C6" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" s="1">
         <v>43389</v>
@@ -816,420 +918,397 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
+        <v>111</v>
+      </c>
+      <c r="C8">
+        <v>2018</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="C9" t="s">
-        <v>61</v>
+        <v>112</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
+        <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>98</v>
+      </c>
+      <c r="B20" t="s">
+        <v>27</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>52</v>
-      </c>
-      <c r="B21" t="s">
-        <v>49</v>
-      </c>
-      <c r="C21" t="s">
-        <v>110</v>
-      </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>53</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>69</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="C23" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>110</v>
+        <v>66</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26">
-        <v>10.6</v>
+        <v>49</v>
+      </c>
+      <c r="C26" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>56</v>
+      </c>
+      <c r="B27" t="s">
+        <v>15</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C28">
-        <v>9.8000000000000007</v>
+        <v>10.6</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
-      </c>
-      <c r="B29" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29">
-        <v>3.7</v>
+        <v>76</v>
+      </c>
+      <c r="C29" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" t="s">
-        <v>107</v>
+        <v>17</v>
+      </c>
+      <c r="C30">
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>69</v>
+        <v>18</v>
+      </c>
+      <c r="C31">
+        <v>3.7</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>47</v>
+      </c>
+      <c r="B32" t="s">
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>73</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>74</v>
+        <v>67</v>
+      </c>
+      <c r="B33" t="s">
+        <v>20</v>
       </c>
       <c r="C33" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C34" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C35" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" t="s">
-        <v>85</v>
+        <v>72</v>
       </c>
       <c r="C36" t="s">
-        <v>83</v>
+        <v>73</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" t="s">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="B38" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C38" t="s">
-        <v>90</v>
+        <v>79</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="B39" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C39" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>95</v>
-      </c>
-      <c r="C41" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>96</v>
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>81</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>99</v>
+        <v>104</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>105</v>
+        <v>92</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="90" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>106</v>
+      </c>
       <c r="B48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>55</v>
+        <v>107</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1240,522 +1319,620 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E56"/>
+  <dimension ref="A1:F53"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C53" sqref="A2:C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.140625" customWidth="1"/>
     <col min="3" max="3" width="42.140625" customWidth="1"/>
     <col min="4" max="4" width="22.42578125" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>42</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="1">
+        <v>43405</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+      <c r="C8">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+      <c r="C9">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>43</v>
       </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>32</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>34</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43389</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>37</v>
       </c>
-      <c r="C9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>38</v>
       </c>
-      <c r="C11" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>39</v>
       </c>
-      <c r="C12" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>40</v>
       </c>
-      <c r="C13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>67</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
       <c r="C16" t="s">
-        <v>69</v>
+        <v>58</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="120" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>28</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>103</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D19" s="2"/>
+        <v>65</v>
+      </c>
+      <c r="B19" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>56</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-      <c r="C20" t="s">
-        <v>60</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="2"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B21" t="s">
-        <v>49</v>
+        <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
-      </c>
-      <c r="C22" t="s">
-        <v>69</v>
+        <v>48</v>
+      </c>
+      <c r="C22">
+        <v>20181016.100000001</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B23" t="s">
-        <v>15</v>
-      </c>
-      <c r="C23" t="s">
-        <v>58</v>
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>3263</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
-      </c>
-      <c r="C25" t="s">
-        <v>69</v>
+        <v>49</v>
+      </c>
+      <c r="C25">
+        <v>20181016.199999999</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C26">
-        <v>10.6</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>80</v>
-      </c>
-      <c r="C27" t="s">
-        <v>81</v>
+        <v>44</v>
+      </c>
+      <c r="B27" t="s">
+        <v>16</v>
+      </c>
+      <c r="C27">
+        <v>10.6</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>46</v>
-      </c>
-      <c r="B28" t="s">
-        <v>18</v>
-      </c>
-      <c r="C28">
-        <v>9.8000000000000007</v>
+        <v>76</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B29" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C29">
-        <v>3.7</v>
+        <v>9.8000000000000007</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B30" t="s">
-        <v>20</v>
-      </c>
-      <c r="C30" t="s">
-        <v>107</v>
+        <v>18</v>
+      </c>
+      <c r="C30">
+        <v>3.7</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="B31" t="s">
-        <v>21</v>
-      </c>
-      <c r="C31" t="s">
-        <v>69</v>
+        <v>19</v>
+      </c>
+      <c r="C31">
+        <v>1.9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>67</v>
+      </c>
+      <c r="B32" t="s">
+        <v>20</v>
+      </c>
+      <c r="C32" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="120" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>72</v>
       </c>
-      <c r="C32" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>74</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="C36" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="C37" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" t="s">
+        <v>81</v>
+      </c>
+      <c r="C38" t="s">
         <v>79</v>
       </c>
-      <c r="C35" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" t="s">
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>80</v>
+      </c>
+      <c r="B39" t="s">
+        <v>81</v>
+      </c>
+      <c r="C39" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>83</v>
+      </c>
+      <c r="B40" t="s">
+        <v>81</v>
+      </c>
+      <c r="C40" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>81</v>
+      </c>
+      <c r="C41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>85</v>
       </c>
-      <c r="C36" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>84</v>
-      </c>
-      <c r="B37" t="s">
-        <v>85</v>
-      </c>
-      <c r="C37" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>87</v>
-      </c>
-      <c r="B38" t="s">
-        <v>85</v>
-      </c>
-      <c r="C38" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>88</v>
-      </c>
-      <c r="B39" t="s">
-        <v>85</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="B42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>89</v>
-      </c>
-      <c r="B40" t="s">
-        <v>85</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D40" s="2" t="s">
+      <c r="C43" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C44" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>96</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>97</v>
-      </c>
-      <c r="C43" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>105</v>
-      </c>
-      <c r="C44" s="2" t="s">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>109</v>
+      </c>
+      <c r="C47" s="2">
         <v>106</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>124</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>106</v>
+      </c>
       <c r="B49" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>55</v>
+        <v>107</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>126</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>120</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A53" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B53" s="4"/>
+      <c r="C53" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="F53" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="58.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Merged PR 1433: Archiving post-deploys, incrementing releases, misc fixes
- Archiving old IRMA post-deploys.  Added missing GO to DeleteRetentionPolicy proc.
- Incrementing IRMA DB version.  Adding new perms for TibcoDataWriter.
- Archiving Mammoth 3.8 post-deploy script.

Related work items: #28706
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\temp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\Icon\DevOps\Release Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="153">
   <si>
     <t>Key</t>
   </si>
@@ -442,25 +442,10 @@
     <t>CHG0033369</t>
   </si>
   <si>
-    <t>CHG0033538</t>
-  </si>
-  <si>
-    <t>Alpesh Patel</t>
-  </si>
-  <si>
-    <t>129 - 130</t>
-  </si>
-  <si>
     <t>RELEASE_2018_12_Sprints129-130</t>
   </si>
   <si>
     <t>10.7.0</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>ExpiringTPRService,MammothPriceListener,R10PriceService,PrimeAffinityListener</t>
   </si>
   <si>
     <t xml:space="preserve"># Valid app-list input: 
@@ -478,6 +463,45 @@
 PrimeAffinityListener   
 R10PriceService         
 </t>
+  </si>
+  <si>
+    <t>131 - 132</t>
+  </si>
+  <si>
+    <t>CHG0034013</t>
+  </si>
+  <si>
+    <t>IRM</t>
+  </si>
+  <si>
+    <t>MammothPriceListener,R10PriceService</t>
+  </si>
+  <si>
+    <t>2.0.1</t>
+  </si>
+  <si>
+    <t>3.8.1</t>
+  </si>
+  <si>
+    <t>9.9.1</t>
+  </si>
+  <si>
+    <t>10.7.1</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_1</t>
+  </si>
+  <si>
+    <t>Mammoth-DB01-QA\Mammoth.Mammoth, QA-01-Mammoth02\Mammoth02.Mammoth</t>
+  </si>
+  <si>
+    <t>MammothDbScriptLink</t>
+  </si>
+  <si>
+    <t>coming soon</t>
+  </si>
+  <si>
+    <t>Using release branch as source, manually upload reports into &lt;a href="http://irmaqarpt/Reports/Pages/Folder.aspx?ItemPath=%2fIcon&amp;ViewMode=Detail"&gt;IIS QA Icon Folder&lt;/a&gt;: Icon IRMA Sign Attributes Comparison.rdl, IconItemSearch.rdl</t>
   </si>
 </sst>
 </file>
@@ -529,7 +553,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -544,7 +568,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -870,11 +893,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -911,7 +934,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -922,7 +945,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>138</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -933,7 +956,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -963,7 +986,7 @@
         <v>9</v>
       </c>
       <c r="C7" s="7">
-        <v>43417</v>
+        <v>43445</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -971,7 +994,7 @@
         <v>108</v>
       </c>
       <c r="C8" s="6">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -979,7 +1002,7 @@
         <v>109</v>
       </c>
       <c r="C9" s="6">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1082,333 +1105,345 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C21" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D21" s="10"/>
+    </row>
+    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="D21" s="11" t="s">
+      <c r="C22" s="10" t="s">
+        <v>149</v>
+      </c>
+      <c r="D22" s="10" t="s">
         <v>99</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>53</v>
-      </c>
-      <c r="B22" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="10">
-        <v>20181108.100000001</v>
+        <v>12</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D23" s="9" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" t="s">
-        <v>65</v>
+        <v>48</v>
+      </c>
+      <c r="C24" s="9">
+        <v>20181210.100000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>14</v>
-      </c>
-      <c r="C25" s="8" t="s">
-        <v>140</v>
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="8">
-        <v>20181112.100000001</v>
+        <v>14</v>
+      </c>
+      <c r="C26" s="9" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B27" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" t="s">
-        <v>65</v>
+        <v>49</v>
+      </c>
+      <c r="C27">
+        <v>20181206.100000001</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="B28" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28">
-        <v>10.7</v>
+        <v>15</v>
+      </c>
+      <c r="C28" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>75</v>
+        <v>44</v>
+      </c>
+      <c r="B29" t="s">
+        <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>141</v>
+        <v>147</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" t="s">
-        <v>17</v>
-      </c>
-      <c r="C30">
-        <v>9.9</v>
+        <v>75</v>
+      </c>
+      <c r="C30" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>18</v>
-      </c>
-      <c r="C31">
-        <v>3.8</v>
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B32" t="s">
-        <v>19</v>
-      </c>
-      <c r="C32" s="12" t="s">
-        <v>142</v>
+        <v>18</v>
+      </c>
+      <c r="C32" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
-        <v>20</v>
-      </c>
-      <c r="C33" t="s">
-        <v>65</v>
+        <v>19</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="B34" t="s">
+        <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C38" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
         <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
         <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
         <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="9" t="s">
+      <c r="C42" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>90</v>
       </c>
-      <c r="C43" s="10" t="s">
+      <c r="C44" s="9" t="s">
         <v>143</v>
       </c>
-      <c r="D43" s="13" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="D44" s="12" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>92</v>
       </c>
-      <c r="C45" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C46" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
         <v>106</v>
       </c>
-      <c r="C47" s="2" t="s">
+      <c r="C48" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="120" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>103</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B49" t="s">
         <v>104</v>
       </c>
-      <c r="C48" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="D48" s="2" t="s">
+      <c r="C49" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="D49" s="2" t="s">
         <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>121</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="F49" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>102</v>
+        <v>142</v>
+      </c>
+      <c r="F50" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+      <c r="A53" t="s">
+        <v>117</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C53" s="5" t="s">
+      <c r="C54" s="5" t="s">
         <v>135</v>
       </c>
     </row>
@@ -1420,11 +1455,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F53"/>
+  <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1776,191 +1811,200 @@
         <v>96</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" t="s">
-        <v>68</v>
-      </c>
+    <row r="34" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>113</v>
+        <v>68</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>74</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>111</v>
+        <v>71</v>
+      </c>
+      <c r="C37" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>77</v>
-      </c>
-      <c r="B38" t="s">
-        <v>80</v>
-      </c>
-      <c r="C38" t="s">
-        <v>78</v>
+        <v>74</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B39" t="s">
         <v>80</v>
       </c>
       <c r="C39" t="s">
-        <v>114</v>
+        <v>78</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
         <v>80</v>
       </c>
       <c r="C40" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B41" t="s">
         <v>80</v>
       </c>
       <c r="C41" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
         <v>80</v>
       </c>
-      <c r="C42" s="2" t="s">
+      <c r="C42" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>84</v>
+      </c>
+      <c r="B43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C43" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="D43" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
         <v>90</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C44" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>91</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="C45" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
         <v>92</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C46" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>100</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>120</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>106</v>
-      </c>
-      <c r="C47" s="2">
-        <v>106</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" s="2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>121</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="50" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
         <v>103</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B50" t="s">
         <v>104</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C50" s="2" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
         <v>123</v>
       </c>
-      <c r="C50" s="2" t="s">
+      <c r="C51" s="2" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>118</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C52" s="2" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
         <v>117</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C53" s="2" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A53" s="4" t="s">
+    <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A54" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="5" t="s">
+      <c r="B54" s="4"/>
+      <c r="C54" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D54" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="F53" t="s">
+      <c r="F54" t="s">
         <v>131</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merged PR 1512: Updated doc-gen script to generate only PN links for new HoneyCrisp TIBCO apps.
Updated doc-gen script to generate only PN links for new HoneyCrisp TIBCO apps.  Setup prod-release doc values.

Related work items: #30866
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="154">
   <si>
     <t>Key</t>
   </si>
@@ -199,9 +199,6 @@
     <t>IrmaBuildId</t>
   </si>
   <si>
-    <t>RELEASE_Icon98_Mammoth37_Sprints127-128</t>
-  </si>
-  <si>
     <t>y</t>
   </si>
   <si>
@@ -211,9 +208,6 @@
     <t>Tom Lux</t>
   </si>
   <si>
-    <t>127-128</t>
-  </si>
-  <si>
     <t>QA</t>
   </si>
   <si>
@@ -305,9 +299,6 @@
   </si>
   <si>
     <t>IrmaSuitePreviousVersion</t>
-  </si>
-  <si>
-    <t>10.5.0</t>
   </si>
   <si>
     <t>If limited or no user downloads, deploy previous version of IRMA Client via VSTS (anyone who downloaded new client, must remove 'apps\2.0\' folder).  If many users downloaded client update, the version should be incremented in Git, then client rebuilt and deployed.</t>
@@ -396,19 +387,10 @@
     <t>AdditionalIrmaDeployImplementerRef</t>
   </si>
   <si>
-    <t>SysMgmt, Apps/Tools</t>
-  </si>
-  <si>
     <t>AdditionalIrmaComponentList</t>
   </si>
   <si>
     <t>Open folder &lt;a href="\\irmaqafile\e$\irma\Staging\Release\Launcher"&gt;Release Launcher Folder&lt;/a&gt;.  Right-click script "IRMA Release Launcher.__IrmaReleaseLauncherVersionRef__.__TargetEnvShort__.ps1" &gt; Run with PowerShell&lt;br&gt;__AdditionalIrmaComponentList__</t>
-  </si>
-  <si>
-    <t>**Components**: IRMA Mobile Plugin (FL-Region Only), WFMUHS</t>
-  </si>
-  <si>
-    <t>MammothActivePriceService</t>
   </si>
   <si>
     <t>QA: CERD1673, CERD1674 | QA-Perf: CERD1662, CERD1663, CERD1664, CERD1665
@@ -437,9 +419,6 @@
   </si>
   <si>
     <t>None, continue</t>
-  </si>
-  <si>
-    <t>CHG0033369</t>
   </si>
   <si>
     <t>RELEASE_2018_12_Sprints129-130</t>
@@ -498,10 +477,34 @@
     <t>MammothDbScriptLink</t>
   </si>
   <si>
-    <t>coming soon</t>
-  </si>
-  <si>
     <t>Using release branch as source, manually upload reports into &lt;a href="http://irmaqarpt/Reports/Pages/Folder.aspx?ItemPath=%2fIcon&amp;ViewMode=Detail"&gt;IIS QA Icon Folder&lt;/a&gt;: Icon IRMA Sign Attributes Comparison.rdl, IconItemSearch.rdl</t>
+  </si>
+  <si>
+    <t>129-132</t>
+  </si>
+  <si>
+    <t>CHG0034401</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_01</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>MammothPriceListener,R10PriceService,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,RePublishInventoryMessagesService</t>
+  </si>
+  <si>
+    <t>IRMA DevOps, DBA</t>
+  </si>
+  <si>
+    <t>**Component Summary**: 'Icon Item Search' SSRS Report, HoneyCrisp SSIS Setup</t>
+  </si>
+  <si>
+    <t>[1 of 2] (IRMA DevOps) Using release branch as source, manually upload report into &lt;a href="http://irmaprdrpt/Reports/Pages/Folder.aspx?ItemPath=%2fIcon&amp;ViewMode=Detail"&gt;IIS Prd Icon Folder&lt;/a&gt;: IconItemSearch.rdl&lt;BR&gt;[2 of 2] (DBA, IRMA DevOps) Open and implement &lt;a href="http://sites/global/ChangeControlDocumentation/Change%20Control%20Documentation/HoneyCrisp%20Prd%20-%20Setup%20ItemVendorLane%20SSIS%20Pkgs.docx"&gt;HoneyCrisp Prod Setup ItemVendorLane SSIS&lt;/a&gt;.&lt;BR&gt;__AdditionalIrmaComponentList__</t>
+  </si>
+  <si>
+    <t>&lt;a href="file://irmaqafile/e$/IRMA/Staging/mammoth/__MammothVer__/DB/Mammoth%20__MammothVer__%20Updates.sql"&gt;Mammoth __MammothVer__ DB Updates&lt;/a&gt;</t>
   </si>
 </sst>
 </file>
@@ -895,9 +898,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -917,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -934,7 +937,7 @@
         <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -945,7 +948,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -956,7 +959,7 @@
         <v>7</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -967,15 +970,15 @@
         <v>8</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -991,7 +994,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C8" s="6">
         <v>2019</v>
@@ -999,7 +1002,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9" s="6">
         <v>1</v>
@@ -1010,7 +1013,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1018,7 +1021,7 @@
         <v>36</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1026,7 +1029,7 @@
         <v>43</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,7 +1037,7 @@
         <v>37</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1042,7 +1045,7 @@
         <v>38</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,7 +1053,7 @@
         <v>39</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1058,7 +1061,7 @@
         <v>40</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1066,63 +1069,63 @@
         <v>34</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B20" t="s">
         <v>27</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D21" s="10"/>
     </row>
     <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1133,10 +1136,10 @@
         <v>12</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1158,7 +1161,7 @@
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1169,7 +1172,7 @@
         <v>14</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1191,7 +1194,7 @@
         <v>15</v>
       </c>
       <c r="C28" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1202,15 +1205,15 @@
         <v>16</v>
       </c>
       <c r="C29" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C30" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,7 +1224,7 @@
         <v>17</v>
       </c>
       <c r="C31" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1232,7 +1235,7 @@
         <v>18</v>
       </c>
       <c r="C32" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1243,208 +1246,208 @@
         <v>19</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B34" t="s">
         <v>20</v>
       </c>
       <c r="C34" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
+        <v>77</v>
+      </c>
+      <c r="B40" t="s">
+        <v>78</v>
+      </c>
+      <c r="C40" t="s">
         <v>79</v>
-      </c>
-      <c r="B40" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
       <c r="D44" s="12" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B49" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="F50" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="5" t="s">
         <v>129</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1457,9 +1460,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C54" sqref="A2:C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1479,7 +1482,7 @@
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -1488,7 +1491,7 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1499,7 +1502,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>136</v>
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1510,7 +1513,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1521,7 +1524,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1532,15 +1535,15 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C6" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1551,23 +1554,23 @@
         <v>9</v>
       </c>
       <c r="C7" s="1">
-        <v>43405</v>
+        <v>43482</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C8">
-        <v>2018</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C9">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1575,7 +1578,7 @@
         <v>35</v>
       </c>
       <c r="C10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1583,7 +1586,7 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1591,7 +1594,7 @@
         <v>43</v>
       </c>
       <c r="C12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1599,7 +1602,7 @@
         <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1607,7 +1610,7 @@
         <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1615,7 +1618,7 @@
         <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1623,7 +1626,7 @@
         <v>40</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1631,37 +1634,37 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
         <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>11</v>
       </c>
       <c r="C19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D20" s="2"/>
     </row>
@@ -1673,7 +1676,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>57</v>
+        <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -1684,7 +1687,7 @@
         <v>48</v>
       </c>
       <c r="C22">
-        <v>20181016.100000001</v>
+        <v>20190110.100000001</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1694,9 +1697,6 @@
       <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C23">
-        <v>3263</v>
-      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
@@ -1716,8 +1716,8 @@
       <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="C25">
-        <v>20181016.199999999</v>
+      <c r="C25" s="9">
+        <v>20190110.100000001</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1727,9 +1727,6 @@
       <c r="B26" t="s">
         <v>15</v>
       </c>
-      <c r="C26">
-        <v>3265</v>
-      </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
@@ -1738,16 +1735,16 @@
       <c r="B27" t="s">
         <v>16</v>
       </c>
-      <c r="C27">
-        <v>10.6</v>
+      <c r="C27" s="11">
+        <v>10.7</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" t="s">
-        <v>76</v>
+        <v>73</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1757,8 +1754,8 @@
       <c r="B29" t="s">
         <v>17</v>
       </c>
-      <c r="C29">
-        <v>9.8000000000000007</v>
+      <c r="C29" s="11">
+        <v>9.9</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1768,8 +1765,8 @@
       <c r="B30" t="s">
         <v>18</v>
       </c>
-      <c r="C30">
-        <v>3.7</v>
+      <c r="C30" s="11">
+        <v>3.8</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1779,233 +1776,242 @@
       <c r="B31" t="s">
         <v>19</v>
       </c>
-      <c r="C31">
-        <v>1.9</v>
+      <c r="C31" s="11" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B32" t="s">
         <v>20</v>
       </c>
       <c r="C32" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B33" t="s">
         <v>27</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C34" s="10" t="s">
-        <v>151</v>
+        <v>143</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="D34" s="10"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B40" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C40" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C41" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C42" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B43" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>90</v>
-      </c>
-      <c r="C44" t="s">
-        <v>126</v>
+        <v>88</v>
+      </c>
+      <c r="C44" s="10" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>89</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>120</v>
+        <v>99</v>
+      </c>
+      <c r="D47" s="10" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>106</v>
-      </c>
-      <c r="C48" s="2">
-        <v>106</v>
+        <v>103</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="225" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B50" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>124</v>
+        <v>152</v>
+      </c>
+      <c r="D50" s="10" t="s">
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>125</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>117</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>132</v>
+        <v>114</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="D53" s="10" t="s">
+        <v>126</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="5" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
       <c r="F54" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 44: Release doc 2019.2 + misc updates
- Initial QA doc for 2019.2
- Consolidated azure-releases section.  Pre, post, and IRMA script have link to new irmaprdfile2 folder, then name of script.  New db-results logs folder.  Moved ReleaseId var to ReleaseInstance and ReleaseId is now dynamic "year.instance"; had to update PS-script refs.
- Loop to update place-holder var refs in input vars 3 times.  Refs to hostname for IRMAPrdFile2.  New template-type vars for DB-update and roll-back scripts.  Updated component list we deployed.

Related work items: #4568
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\Icon\DevOps\Release Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\scad\DevOps\Release Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,10 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="154">
-  <si>
-    <t>Key</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="165">
   <si>
     <t>Template</t>
   </si>
@@ -410,9 +407,6 @@
   </si>
   <si>
     <t>&lt;hr&gt;Additional special-fixes build, 'RELEASE_FastTrack_Sprints127-128' branch, build=20181030.1</t>
-  </si>
-  <si>
-    <t>&lt;a href="file://irmaqafile/e$/IRMA/Staging/iCon/__IconVer__/DB/Icon%20__IconVer__%20Updates.sql"&gt;Icon __IconVer__ DB Updates&lt;/a&gt;</t>
   </si>
   <si>
     <t>&lt;span style='background:lime;mso-highlight:lime'&gt;**Start Price-Batch Purge ASAP** (see separate doc)&lt;/span&gt;</t>
@@ -444,42 +438,15 @@
 </t>
   </si>
   <si>
-    <t>131 - 132</t>
-  </si>
-  <si>
-    <t>CHG0034013</t>
-  </si>
-  <si>
     <t>IRM</t>
   </si>
   <si>
-    <t>MammothPriceListener,R10PriceService</t>
-  </si>
-  <si>
-    <t>2.0.1</t>
-  </si>
-  <si>
-    <t>3.8.1</t>
-  </si>
-  <si>
-    <t>9.9.1</t>
-  </si>
-  <si>
-    <t>10.7.1</t>
-  </si>
-  <si>
-    <t>RELEASE_2019_1</t>
-  </si>
-  <si>
     <t>Mammoth-DB01-QA\Mammoth.Mammoth, QA-01-Mammoth02\Mammoth02.Mammoth</t>
   </si>
   <si>
     <t>MammothDbScriptLink</t>
   </si>
   <si>
-    <t>Using release branch as source, manually upload reports into &lt;a href="http://irmaqarpt/Reports/Pages/Folder.aspx?ItemPath=%2fIcon&amp;ViewMode=Detail"&gt;IIS QA Icon Folder&lt;/a&gt;: Icon IRMA Sign Attributes Comparison.rdl, IconItemSearch.rdl</t>
-  </si>
-  <si>
     <t>129-132</t>
   </si>
   <si>
@@ -505,6 +472,72 @@
   </si>
   <si>
     <t>&lt;a href="file://irmaqafile/e$/IRMA/Staging/mammoth/__MammothVer__/DB/Mammoth%20__MammothVer__%20Updates.sql"&gt;Mammoth __MammothVer__ DB Updates&lt;/a&gt;</t>
+  </si>
+  <si>
+    <t>CHG0035179</t>
+  </si>
+  <si>
+    <t>133 - 136</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_2</t>
+  </si>
+  <si>
+    <t>10.8.0</t>
+  </si>
+  <si>
+    <t>2.1</t>
+  </si>
+  <si>
+    <t>EslPriceListener,OnePlumPriceListener</t>
+  </si>
+  <si>
+    <t>10.0</t>
+  </si>
+  <si>
+    <t>__ReleaseYear__.__ReleaseInstance__</t>
+  </si>
+  <si>
+    <t>ReleaseInstance</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;icon.db&lt;br&gt;mammoth.db&lt;br&gt;irma client&lt;br&gt;icon/api controller&lt;br&gt;icon/web/&lt;br&gt;/mammothauditservice&lt;br&gt;mammoth/esb/.*locale&lt;br&gt;mammothwebapi&lt;br&gt;mammoth/websupport</t>
+  </si>
+  <si>
+    <t>Open Folder HERE, FileName: IRMA __ReleaseId__ Updates.sql</t>
+  </si>
+  <si>
+    <t>Open Folder &lt;a href="file://odwp6516/Release/__ReleaseId__/"&gt;HERE&lt;/a&gt;, FileName: &lt;span style='background:#A8D08D;mso-shading-themecolor:accent6;mso-shading-themetint:153'&gt;IRMA __ReleaseId__ Updates.sql&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Open Folder &lt;a href="file://odwp6516/Release/__ReleaseId__/"&gt;HERE&lt;/a&gt;, FileName: &lt;span style='background:#A8D08D;mso-shading-themecolor:accent6;mso-shading-themetint:153'&gt;Icon __ReleaseId__ Updates.sql&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Open Folder &lt;a href="file://odwp6516/Release/__ReleaseId__/"&gt;HERE&lt;/a&gt;, FileName: &lt;span style='background:#A8D08D;mso-shading-themecolor:accent6;mso-shading-themetint:153'&gt;Mammoth __ReleaseId__ Updates.sql&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>IrmaDbScriptLink</t>
+  </si>
+  <si>
+    <t>IrmaDbRollBackScriptLink</t>
+  </si>
+  <si>
+    <t>IconDbRollBackScriptLink</t>
+  </si>
+  <si>
+    <t>MammothDbRollBackScriptLink</t>
+  </si>
+  <si>
+    <t>Open Folder &lt;a href="file://odwp6516/Release/__ReleaseId__/"&gt;HERE&lt;/a&gt;, FileName: &lt;span style='background:#A8D08D;mso-shading-themecolor:accent6;mso-shading-themetint:153'&gt;IRMA __ReleaseId__ Updates__ROLL-BACK.sql&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Open Folder &lt;a href="file://odwp6516/Release/__ReleaseId__/"&gt;HERE&lt;/a&gt;, FileName: &lt;span style='background:#A8D08D;mso-shading-themecolor:accent6;mso-shading-themetint:153'&gt;Icon __ReleaseId__ Updates__ROLL-BACK.sql&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Open Folder &lt;a href="file://odwp6516/Release/__ReleaseId__/"&gt;HERE&lt;/a&gt;, FileName: &lt;span style='background:#A8D08D;mso-shading-themecolor:accent6;mso-shading-themetint:153'&gt;Mammoth __ReleaseId__ Updates__ROLL-BACK.sql&lt;/span&gt;</t>
+  </si>
+  <si>
+    <t>Key (**WARNING: Case-Sensitive**)</t>
   </si>
 </sst>
 </file>
@@ -896,11 +929,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A48" sqref="A48"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,87 +947,87 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="7">
-        <v>43445</v>
+        <v>43501</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8" s="6">
         <v>2019</v>
@@ -1002,39 +1035,39 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>106</v>
+        <v>151</v>
       </c>
       <c r="C9" s="6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>57</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>57</v>
@@ -1042,115 +1075,106 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
-      </c>
-      <c r="C18" t="s">
-        <v>63</v>
+        <v>33</v>
+      </c>
+      <c r="C18" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>93</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D23" s="10"/>
+    </row>
+    <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>94</v>
       </c>
-      <c r="B20" t="s">
-        <v>27</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="10"/>
-    </row>
-    <row r="22" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C24" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>95</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="D22" s="10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>53</v>
-      </c>
-      <c r="B23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C23" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="D23" s="9" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="9">
-        <v>20181210.100000001</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1158,296 +1182,345 @@
         <v>52</v>
       </c>
       <c r="B25" t="s">
-        <v>13</v>
-      </c>
-      <c r="C25" t="s">
-        <v>63</v>
+        <v>11</v>
+      </c>
+      <c r="C25" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="9" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B26" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="9" t="s">
-        <v>141</v>
+        <v>47</v>
+      </c>
+      <c r="C26" s="11">
+        <v>20181210.100000001</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C27">
-        <v>20181206.100000001</v>
+        <v>12</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s">
-        <v>15</v>
-      </c>
-      <c r="C28" t="s">
-        <v>63</v>
+        <v>13</v>
+      </c>
+      <c r="C28" s="11" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B29" t="s">
-        <v>16</v>
-      </c>
-      <c r="C29" t="s">
-        <v>140</v>
+        <v>48</v>
+      </c>
+      <c r="C29" s="11">
+        <v>20181206.100000001</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" t="s">
-        <v>140</v>
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30" s="11" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>17</v>
-      </c>
-      <c r="C31" t="s">
-        <v>139</v>
+        <v>15</v>
+      </c>
+      <c r="C31" s="11">
+        <v>10.8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>46</v>
-      </c>
-      <c r="B32" t="s">
-        <v>18</v>
-      </c>
-      <c r="C32" t="s">
-        <v>138</v>
+        <v>72</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B33" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>64</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>20</v>
-      </c>
-      <c r="C34" t="s">
-        <v>63</v>
+        <v>17</v>
+      </c>
+      <c r="C34" s="11">
+        <v>3.9</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="11" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="B36" t="s">
+        <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C37" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="C40" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B41" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C41" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
         <v>81</v>
       </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="8" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>85</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+      <c r="D45" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
         <v>88</v>
       </c>
-      <c r="C44" s="9" t="s">
-        <v>136</v>
-      </c>
-      <c r="D44" s="12" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+      <c r="C47" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="C46" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B49" t="s">
-        <v>101</v>
-      </c>
-      <c r="C49" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>102</v>
+        <v>96</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="F50" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>99</v>
+      </c>
+      <c r="B51" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>99</v>
+      <c r="C51" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>116</v>
+        <v>131</v>
+      </c>
+      <c r="F52" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
         <v>114</v>
       </c>
-      <c r="C53" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>129</v>
+      <c r="C54" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -1458,100 +1531,100 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C54" sqref="A2:C54"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.140625" customWidth="1"/>
-    <col min="3" max="3" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
       <c r="F1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>135</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C7" s="1">
         <v>43482</v>
@@ -1559,459 +1632,504 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C8">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>106</v>
-      </c>
-      <c r="C9">
+    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" s="9">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" t="s">
-        <v>57</v>
+    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18" t="s">
-        <v>10</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" t="s">
         <v>62</v>
-      </c>
-      <c r="B19" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="D20" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="B20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>53</v>
-      </c>
-      <c r="B21" t="s">
-        <v>12</v>
-      </c>
-      <c r="C21" t="s">
-        <v>147</v>
-      </c>
+        <v>94</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="2"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C22">
-        <v>20190110.100000001</v>
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>13</v>
+        <v>47</v>
+      </c>
+      <c r="C23">
+        <v>20190110.100000001</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" t="s">
-        <v>55</v>
+        <v>12</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
-      </c>
-      <c r="C25" s="9">
-        <v>20190110.100000001</v>
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B26" t="s">
-        <v>15</v>
+        <v>48</v>
+      </c>
+      <c r="C26" s="9">
+        <v>20190110.100000001</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="B27" t="s">
-        <v>16</v>
-      </c>
-      <c r="C27" s="11">
-        <v>10.7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C28" s="11" t="s">
-        <v>131</v>
+        <v>43</v>
+      </c>
+      <c r="B28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="11">
+        <v>10.7</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>45</v>
-      </c>
-      <c r="B29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C29" s="11">
-        <v>9.9</v>
+        <v>72</v>
+      </c>
+      <c r="C29" s="11" t="s">
+        <v>129</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B30" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C30" s="11">
-        <v>3.8</v>
+        <v>9.9</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
-      </c>
-      <c r="C31" s="11" t="s">
-        <v>148</v>
+        <v>17</v>
+      </c>
+      <c r="C31" s="11">
+        <v>3.8</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>63</v>
+      </c>
+      <c r="B33" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="9" t="s">
+        <v>157</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>64</v>
       </c>
-      <c r="B32" t="s">
-        <v>20</v>
-      </c>
-      <c r="C32" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" ht="90" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="3" t="s">
+      <c r="C37" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>66</v>
+      </c>
+      <c r="C38" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>71</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" t="s">
+        <v>77</v>
+      </c>
+      <c r="C41" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" t="s">
+        <v>77</v>
+      </c>
+      <c r="C42" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43" t="s">
+        <v>77</v>
+      </c>
+      <c r="C43" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>80</v>
+      </c>
+      <c r="B44" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>81</v>
+      </c>
+      <c r="B45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>87</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>88</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>89</v>
+      </c>
+      <c r="C48" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" s="10" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>102</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>117</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>118</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>114</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="D55" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A56" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B56" s="4"/>
+      <c r="C56" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="9" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="D34" s="10"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>65</v>
-      </c>
-      <c r="C35" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>67</v>
-      </c>
-      <c r="C36" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="C37" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>72</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" t="s">
-        <v>78</v>
-      </c>
-      <c r="C39" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>77</v>
-      </c>
-      <c r="B40" t="s">
-        <v>78</v>
-      </c>
-      <c r="C40" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>81</v>
-      </c>
-      <c r="B42" t="s">
-        <v>78</v>
-      </c>
-      <c r="C42" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>82</v>
-      </c>
-      <c r="B43" t="s">
-        <v>78</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>89</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>97</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>103</v>
-      </c>
-      <c r="C48" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>118</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="225" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>100</v>
-      </c>
-      <c r="B50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>119</v>
-      </c>
-      <c r="C51" s="2" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>115</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>114</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>116</v>
-      </c>
-      <c r="D53" s="10" t="s">
+      <c r="D56" s="5" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A54" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F54" t="s">
-        <v>125</v>
+      <c r="F56" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A57" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A58" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>163</v>
       </c>
     </row>
   </sheetData>
@@ -2035,52 +2153,52 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 79: Prod reldoc for 2019.2 release.  Updates to release-prep section to cover new
Prod reldoc for 2019.2 release.  Updates to release-prep section to cover new individual-releases format to deliver apps from Azure.

Related work items: #4915
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="163">
   <si>
     <t>Template</t>
   </si>
@@ -245,9 +245,6 @@
   </si>
   <si>
     <t>IrmaLongVer</t>
-  </si>
-  <si>
-    <t>10.6.0</t>
   </si>
   <si>
     <t>AppSuitesBeingDeployed</t>
@@ -363,9 +360,6 @@
     <t>IRMAPrdApp[1-8]</t>
   </si>
   <si>
-    <t>Mammoth-App01-QA, IRMAPrdApp[9-10]</t>
-  </si>
-  <si>
     <t>VM-Icon-Prd[1-6]</t>
   </si>
   <si>
@@ -385,9 +379,6 @@
   </si>
   <si>
     <t>AdditionalIrmaComponentList</t>
-  </si>
-  <si>
-    <t>Open folder &lt;a href="\\irmaqafile\e$\irma\Staging\Release\Launcher"&gt;Release Launcher Folder&lt;/a&gt;.  Right-click script "IRMA Release Launcher.__IrmaReleaseLauncherVersionRef__.__TargetEnvShort__.ps1" &gt; Run with PowerShell&lt;br&gt;__AdditionalIrmaComponentList__</t>
   </si>
   <si>
     <t>QA: CERD1673, CERD1674 | QA-Perf: CERD1662, CERD1663, CERD1664, CERD1665
@@ -447,27 +438,9 @@
     <t>MammothDbScriptLink</t>
   </si>
   <si>
-    <t>129-132</t>
-  </si>
-  <si>
-    <t>CHG0034401</t>
-  </si>
-  <si>
-    <t>RELEASE_2019_01</t>
-  </si>
-  <si>
-    <t>2.0</t>
-  </si>
-  <si>
     <t>MammothPriceListener,R10PriceService,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,RePublishInventoryMessagesService</t>
   </si>
   <si>
-    <t>IRMA DevOps, DBA</t>
-  </si>
-  <si>
-    <t>**Component Summary**: 'Icon Item Search' SSRS Report, HoneyCrisp SSIS Setup</t>
-  </si>
-  <si>
     <t>[1 of 2] (IRMA DevOps) Using release branch as source, manually upload report into &lt;a href="http://irmaprdrpt/Reports/Pages/Folder.aspx?ItemPath=%2fIcon&amp;ViewMode=Detail"&gt;IIS Prd Icon Folder&lt;/a&gt;: IconItemSearch.rdl&lt;BR&gt;[2 of 2] (DBA, IRMA DevOps) Open and implement &lt;a href="http://sites/global/ChangeControlDocumentation/Change%20Control%20Documentation/HoneyCrisp%20Prd%20-%20Setup%20ItemVendorLane%20SSIS%20Pkgs.docx"&gt;HoneyCrisp Prod Setup ItemVendorLane SSIS&lt;/a&gt;.&lt;BR&gt;__AdditionalIrmaComponentList__</t>
   </si>
   <si>
@@ -538,6 +511,27 @@
   </si>
   <si>
     <t>Key (**WARNING: Case-Sensitive**)</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>Mammoth-App01-Prd, IRMAPrdApp[9-10]</t>
+  </si>
+  <si>
+    <t>CHG0035645</t>
+  </si>
+  <si>
+    <t>EslPriceListener,OnePlumPriceListener,MammothPriceListener</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;irma client&lt;br&gt;icon/api controller&lt;br&gt;icon/web/&lt;br&gt;mammoth/esb/.*locale&lt;br&gt;mammothwebapi&lt;br&gt;mammoth/websupport</t>
+  </si>
+  <si>
+    <t>Open folder &lt;a href="\\irmaprdfile2\e$\Release\2019.2\"&gt;Release Launcher Folder&lt;/a&gt;.  Right-click script "Deploy WFMUHS Update.PRD.ps1" &gt; Run with PowerShell&lt;BR&gt;__AdditionalIrmaComponentList__</t>
+  </si>
+  <si>
+    <t>*IRMA Components Deployed By This Script:&lt;br&gt;WFM Mobile Config (11 Regions Code-128 Update)</t>
   </si>
 </sst>
 </file>
@@ -931,9 +925,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A48" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C59" sqref="C59"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -947,13 +941,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -970,7 +964,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -992,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1008,7 +1002,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>59</v>
@@ -1027,7 +1021,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8" s="6">
         <v>2019</v>
@@ -1035,7 +1029,7 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C9" s="6">
         <v>2</v>
@@ -1043,10 +1037,10 @@
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1137,44 +1131,44 @@
     </row>
     <row r="21" spans="1:4" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>93</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>94</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1185,10 +1179,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,7 +1215,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1262,7 +1256,7 @@
         <v>72</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1273,7 +1267,7 @@
         <v>16</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,7 +1289,7 @@
         <v>18</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -1343,100 +1337,100 @@
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" t="s">
         <v>74</v>
-      </c>
-      <c r="B41" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
         <v>76</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>77</v>
-      </c>
-      <c r="C42" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
+        <v>95</v>
+      </c>
+      <c r="C49" s="2" t="s">
         <v>96</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>62</v>
@@ -1444,83 +1438,83 @@
     </row>
     <row r="51" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" t="s">
         <v>99</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="F52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="55" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -1533,8 +1527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F59"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1545,17 +1539,18 @@
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="6" max="6" width="38.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1564,7 +1559,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1575,7 +1570,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1596,8 +1591,8 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" t="s">
-        <v>134</v>
+      <c r="C4" s="9" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1608,15 +1603,15 @@
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,12 +1622,12 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>43482</v>
+        <v>43517</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C8">
         <v>2019</v>
@@ -1640,18 +1635,18 @@
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C9" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1742,10 +1737,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -1768,7 +1763,7 @@
         <v>47</v>
       </c>
       <c r="C23">
-        <v>20190110.100000001</v>
+        <v>20190205.800000001</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1797,8 +1792,8 @@
       <c r="B26" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="9">
-        <v>20190110.100000001</v>
+      <c r="C26" s="9" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1817,7 +1812,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="11">
-        <v>10.7</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1825,7 +1820,7 @@
         <v>72</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1835,8 +1830,8 @@
       <c r="B30" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="11">
-        <v>9.9</v>
+      <c r="C30" s="11" t="s">
+        <v>140</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1847,7 +1842,7 @@
         <v>17</v>
       </c>
       <c r="C31" s="11">
-        <v>3.8</v>
+        <v>3.9</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1858,7 +1853,7 @@
         <v>18</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1874,41 +1869,41 @@
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B35" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>92</v>
-      </c>
       <c r="F35" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>133</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>156</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1924,7 +1919,7 @@
         <v>66</v>
       </c>
       <c r="C38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1932,7 +1927,7 @@
         <v>68</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1940,105 +1935,108 @@
         <v>71</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>73</v>
+      </c>
+      <c r="B41" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" t="s">
         <v>74</v>
-      </c>
-      <c r="B41" t="s">
-        <v>77</v>
-      </c>
-      <c r="C41" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B42" t="s">
         <v>76</v>
       </c>
-      <c r="B42" t="s">
-        <v>77</v>
-      </c>
       <c r="C42" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C43" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C44" t="s">
-        <v>111</v>
+        <v>157</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>87</v>
-      </c>
-      <c r="C46" s="10" t="s">
-        <v>138</v>
+        <v>86</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>159</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C48" t="s">
-        <v>73</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>62</v>
@@ -2046,95 +2044,98 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="285" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>98</v>
+      </c>
+      <c r="B52" t="s">
         <v>99</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="F52" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="C52" s="2" t="s">
-        <v>141</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>118</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>140</v>
+        <v>116</v>
+      </c>
+      <c r="C53" s="10" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>115</v>
+        <v>160</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="5" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="F56" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="57" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Merged PR 500: Cleanup and updates for new sections in release doc template + 2019.05 QA values
- starting new sections but got pulled away
- Rel Doc Input-Spreadsheet Template Updates:
- changed ReleaseInstance to ReleaseSeqNum and ReleaseId now contains the combined year+seq values
- new sections before and after the main 3 DB-update sections
- new placeholder vars: DbBeforeRelScripts, DbAfterRelScripts
- moved azure release table to new section after all DB sections
- changed SpecialIconReleaseDetails to AzureReleaseList in spreadsheet and template
Rel Doc Script:
Changed to use ReleaseId input value because it's combined year & seq num.
- Fixed rel-inst var in title of doc templace (it's now rel-id var).  Moved azure section after tibco section.  Hard-coded tibco-link-generation to be for SO region only (was only PN).
- TOC update
- 2019.05 QA values

Related work items: #5401
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="176">
   <si>
     <t>Template</t>
   </si>
@@ -188,9 +188,6 @@
   </si>
   <si>
     <t>IrmaReleaseBranchName</t>
-  </si>
-  <si>
-    <t>RELEASE_IRMA106_Sprints127-128</t>
   </si>
   <si>
     <t>IrmaBuildId</t>
@@ -363,9 +360,6 @@
     <t>VM-Icon-Prd[1-6]</t>
   </si>
   <si>
-    <t>SpecialIconReleaseDetails</t>
-  </si>
-  <si>
     <t>SpecialIrmaReleaseDetails</t>
   </si>
   <si>
@@ -407,9 +401,6 @@
   </si>
   <si>
     <t>RELEASE_2018_12_Sprints129-130</t>
-  </si>
-  <si>
-    <t>10.7.0</t>
   </si>
   <si>
     <t xml:space="preserve"># Valid app-list input: 
@@ -441,42 +432,9 @@
     <t>MammothPriceListener,R10PriceService,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,RePublishInventoryMessagesService</t>
   </si>
   <si>
-    <t>[1 of 2] (IRMA DevOps) Using release branch as source, manually upload report into &lt;a href="http://irmaprdrpt/Reports/Pages/Folder.aspx?ItemPath=%2fIcon&amp;ViewMode=Detail"&gt;IIS Prd Icon Folder&lt;/a&gt;: IconItemSearch.rdl&lt;BR&gt;[2 of 2] (DBA, IRMA DevOps) Open and implement &lt;a href="http://sites/global/ChangeControlDocumentation/Change%20Control%20Documentation/HoneyCrisp%20Prd%20-%20Setup%20ItemVendorLane%20SSIS%20Pkgs.docx"&gt;HoneyCrisp Prod Setup ItemVendorLane SSIS&lt;/a&gt;.&lt;BR&gt;__AdditionalIrmaComponentList__</t>
-  </si>
-  <si>
     <t>&lt;a href="file://irmaqafile/e$/IRMA/Staging/mammoth/__MammothVer__/DB/Mammoth%20__MammothVer__%20Updates.sql"&gt;Mammoth __MammothVer__ DB Updates&lt;/a&gt;</t>
   </si>
   <si>
-    <t>CHG0035179</t>
-  </si>
-  <si>
-    <t>133 - 136</t>
-  </si>
-  <si>
-    <t>RELEASE_2019_2</t>
-  </si>
-  <si>
-    <t>10.8.0</t>
-  </si>
-  <si>
-    <t>2.1</t>
-  </si>
-  <si>
-    <t>EslPriceListener,OnePlumPriceListener</t>
-  </si>
-  <si>
-    <t>10.0</t>
-  </si>
-  <si>
-    <t>__ReleaseYear__.__ReleaseInstance__</t>
-  </si>
-  <si>
-    <t>ReleaseInstance</t>
-  </si>
-  <si>
-    <t>&lt;hr&gt;icon.db&lt;br&gt;mammoth.db&lt;br&gt;irma client&lt;br&gt;icon/api controller&lt;br&gt;icon/web/&lt;br&gt;/mammothauditservice&lt;br&gt;mammoth/esb/.*locale&lt;br&gt;mammothwebapi&lt;br&gt;mammoth/websupport</t>
-  </si>
-  <si>
     <t>Open Folder HERE, FileName: IRMA __ReleaseId__ Updates.sql</t>
   </si>
   <si>
@@ -519,19 +477,100 @@
     <t>Mammoth-App01-Prd, IRMAPrdApp[9-10]</t>
   </si>
   <si>
-    <t>CHG0035645</t>
-  </si>
-  <si>
-    <t>EslPriceListener,OnePlumPriceListener,MammothPriceListener</t>
-  </si>
-  <si>
-    <t>&lt;hr&gt;irma client&lt;br&gt;icon/api controller&lt;br&gt;icon/web/&lt;br&gt;mammoth/esb/.*locale&lt;br&gt;mammothwebapi&lt;br&gt;mammoth/websupport</t>
-  </si>
-  <si>
-    <t>Open folder &lt;a href="\\irmaprdfile2\e$\Release\2019.2\"&gt;Release Launcher Folder&lt;/a&gt;.  Right-click script "Deploy WFMUHS Update.PRD.ps1" &gt; Run with PowerShell&lt;BR&gt;__AdditionalIrmaComponentList__</t>
-  </si>
-  <si>
-    <t>*IRMA Components Deployed By This Script:&lt;br&gt;WFM Mobile Config (11 Regions Code-128 Update)</t>
+    <t>DbAfterRelScripts</t>
+  </si>
+  <si>
+    <t>**NONE**</t>
+  </si>
+  <si>
+    <t>Full section for DB updates after the core/base release scripts run by DBA.</t>
+  </si>
+  <si>
+    <t>DbBeforeRelScripts</t>
+  </si>
+  <si>
+    <t>Full section for DB updates before the core/base release scripts run by DBA.</t>
+  </si>
+  <si>
+    <t>139 - 140 (Feb 27 - Mar 27)</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_04</t>
+  </si>
+  <si>
+    <t>20190417.*</t>
+  </si>
+  <si>
+    <t>11.0</t>
+  </si>
+  <si>
+    <t>11.0.0</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>AzureReleaseList</t>
+  </si>
+  <si>
+    <t>10.9.0</t>
+  </si>
+  <si>
+    <t>CHG0037090</t>
+  </si>
+  <si>
+    <t>ReleaseSeqNum</t>
+  </si>
+  <si>
+    <t>__ReleaseYear__.__ReleaseSeqNum__</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Infor Item Listener&lt;br&gt;Icon Global Event Controller&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth API Controller&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>PublishReceivedOrderService</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_05</t>
+  </si>
+  <si>
+    <t>20190405*</t>
+  </si>
+  <si>
+    <t>11.1</t>
+  </si>
+  <si>
+    <t>11.1.0</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;eWIC APL Listener&lt;br&gt;eWIC Error-Response Listener&lt;br&gt;Icon API Controller&lt;br&gt;Icon Dashboard&lt;br&gt;Icon Global Event Controller&lt;br&gt;Icon Item-Movement Listener&lt;br&gt;Icon Monitoring Service&lt;br&gt;Icon Nutrition Web API&lt;br&gt;Icon POS Push Controller&lt;br&gt;Icon R10 Listener&lt;br&gt;Icon TLog Controller&lt;br&gt;Icon VIM Locale Controller&lt;br&gt;Icon Web&lt;br&gt;Icon Web API&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth API Controller&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Price Controller&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>CHG0037346</t>
+  </si>
+  <si>
+    <t>141 - 142</t>
+  </si>
+  <si>
+    <t>ActivePriceArchiver,EmergencyPriceService,ErrorMessagesListener,ErrorMessagesMonitor,EslPriceListener,ExpiringTprService,InStockDequeueService,IrmaPriceListener,JobSchedulerService,LoggingService,MammothActivePriceService,MammothPriceListener,OnePlumPriceListener,PriceListenerMessageArchiver,PrimeAffinityListener,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,R10PriceService</t>
+  </si>
+  <si>
+    <t>HcGenerateQafLinks</t>
+  </si>
+  <si>
+    <t>HcTibcoRegions</t>
+  </si>
+  <si>
+    <t>PN,SO,SW</t>
+  </si>
+  <si>
+    <t>List of regions for which tibco deploy links should be generated for HoneyCrisp apps</t>
+  </si>
+  <si>
+    <t>Flag 0 or 1 to indicate if QAF links should be generated for HoneyCrisp tibco apps</t>
   </si>
 </sst>
 </file>
@@ -583,7 +622,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -609,6 +648,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -923,11 +963,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -941,13 +981,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -964,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>134</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -975,7 +1015,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -986,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>135</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -997,15 +1037,15 @@
         <v>7</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1016,31 +1056,34 @@
         <v>8</v>
       </c>
       <c r="C7" s="7">
-        <v>43501</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>103</v>
-      </c>
-      <c r="C8" s="6">
+        <v>43587</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="10"/>
+      <c r="C8" s="9">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="6">
-        <v>2</v>
+    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>158</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>104</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B10" s="10"/>
       <c r="C10" s="9" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1048,7 +1091,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,7 +1099,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1064,7 +1107,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1072,7 +1115,7 @@
         <v>36</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1080,7 +1123,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1088,7 +1131,7 @@
         <v>38</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1096,7 +1139,7 @@
         <v>39</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,71 +1147,71 @@
         <v>33</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B20" t="s">
         <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D23" s="10"/>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="D24" s="10" t="s">
         <v>93</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="D24" s="10" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1179,10 +1222,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>136</v>
+        <v>163</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1192,8 +1235,8 @@
       <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="11">
-        <v>20181210.100000001</v>
+      <c r="C26" s="11" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1204,7 +1247,7 @@
         <v>12</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -1215,7 +1258,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>136</v>
+        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1225,19 +1268,19 @@
       <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="11">
-        <v>20181206.100000001</v>
+      <c r="C29" s="11" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" t="s">
         <v>14</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -1247,16 +1290,16 @@
       <c r="B31" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="11">
-        <v>10.8</v>
+      <c r="C31" s="11" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>137</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,8 +1309,9 @@
       <c r="B33" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="11" t="s">
-        <v>140</v>
+      <c r="C33" s="13" t="str">
+        <f>C10</f>
+        <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -1277,8 +1321,9 @@
       <c r="B34" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="11">
-        <v>3.9</v>
+      <c r="C34" s="13" t="str">
+        <f>C10</f>
+        <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -1288,233 +1333,280 @@
       <c r="B35" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="11" t="s">
-        <v>138</v>
+      <c r="C35" s="13" t="str">
+        <f>C10</f>
+        <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B36" t="s">
         <v>19</v>
       </c>
       <c r="C36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
         <v>64</v>
-      </c>
-      <c r="C37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
         <v>66</v>
-      </c>
-      <c r="C38" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>67</v>
+      </c>
+      <c r="C39" t="s">
         <v>68</v>
-      </c>
-      <c r="C39" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
         <v>73</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" t="s">
         <v>75</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>76</v>
-      </c>
-      <c r="C42" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C44" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B45" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C45" s="8" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="D46" s="12" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" s="12"/>
+    </row>
+    <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0</v>
+      </c>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>139</v>
-      </c>
-      <c r="D46" s="12" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C49" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C48" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="C50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>98</v>
-      </c>
-      <c r="B51" t="s">
-        <v>99</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>100</v>
+        <v>94</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>115</v>
+        <v>100</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="F52" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>97</v>
+      </c>
+      <c r="B53" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>116</v>
-      </c>
-      <c r="C53" s="2" t="s">
-        <v>97</v>
+      <c r="C53" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D53" s="2" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+      <c r="F54" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" ht="330" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1525,17 +1617,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F59"/>
+  <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" customWidth="1"/>
+    <col min="2" max="2" width="58.140625" style="10" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
@@ -1544,13 +1636,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1559,66 +1651,66 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="10" t="s">
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="10" t="s">
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>135</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="1">
@@ -1627,7 +1719,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C8">
         <v>2019</v>
@@ -1635,18 +1727,20 @@
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>142</v>
-      </c>
-      <c r="C9" s="9">
-        <v>2</v>
+        <v>158</v>
+      </c>
+      <c r="B9" s="10"/>
+      <c r="C9" s="11" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>104</v>
-      </c>
+        <v>103</v>
+      </c>
+      <c r="B10" s="10"/>
       <c r="C10" s="9" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1654,7 +1748,7 @@
         <v>34</v>
       </c>
       <c r="C11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,7 +1756,7 @@
         <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1670,7 +1764,7 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1678,7 +1772,7 @@
         <v>36</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1686,7 +1780,7 @@
         <v>37</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1694,7 +1788,7 @@
         <v>38</v>
       </c>
       <c r="C16" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1702,7 +1796,7 @@
         <v>39</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1710,37 +1804,37 @@
         <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>60</v>
-      </c>
-      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" t="s">
         <v>61</v>
-      </c>
-      <c r="B20" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -1748,29 +1842,29 @@
       <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>136</v>
+        <v>150</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C23">
-        <v>20190205.800000001</v>
+      <c r="C23" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B24" s="10" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1778,29 +1872,29 @@
       <c r="A25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B25" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>49</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B26" s="10" t="s">
         <v>48</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>55</v>
-      </c>
-      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="10" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1808,329 +1902,381 @@
       <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B28" t="s">
+      <c r="B28" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="11">
-        <v>10.8</v>
+      <c r="C28" s="11" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B30" t="s">
+      <c r="B30" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="11" t="s">
-        <v>140</v>
+      <c r="C30" s="13" t="str">
+        <f>C10</f>
+        <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="B31" t="s">
+      <c r="B31" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="11">
-        <v>3.9</v>
+      <c r="C31" s="13" t="str">
+        <f>C10</f>
+        <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B32" t="s">
+      <c r="B32" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="11" t="s">
-        <v>138</v>
+      <c r="C32" s="13" t="str">
+        <f>C10</f>
+        <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>63</v>
-      </c>
-      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+      <c r="B33" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C33" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>148</v>
-      </c>
+        <v>134</v>
+      </c>
+      <c r="B34" s="10"/>
       <c r="C34" s="3" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>92</v>
-      </c>
-      <c r="B35" t="s">
+        <v>91</v>
+      </c>
+      <c r="B35" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
       <c r="D35" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E35" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>91</v>
-      </c>
       <c r="F35" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>130</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="B36" s="10"/>
       <c r="C36" s="3" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" t="s">
         <v>64</v>
-      </c>
-      <c r="C37" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>72</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="C41" t="s">
         <v>73</v>
-      </c>
-      <c r="B41" t="s">
-        <v>76</v>
-      </c>
-      <c r="C41" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>74</v>
+      </c>
+      <c r="B42" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B42" t="s">
-        <v>76</v>
-      </c>
       <c r="C42" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>78</v>
-      </c>
-      <c r="B43" t="s">
-        <v>76</v>
+        <v>77</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>79</v>
-      </c>
-      <c r="B44" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="C44" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45" t="s">
-        <v>76</v>
+        <v>79</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
+        <v>85</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="9" t="s">
+        <v>172</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="C47" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47" s="12"/>
+    </row>
+    <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="C48" s="9">
+        <v>0</v>
+      </c>
+      <c r="D48" s="12"/>
+    </row>
+    <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
         <v>86</v>
       </c>
-      <c r="C46" s="9" t="s">
-        <v>159</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>87</v>
-      </c>
-      <c r="C47" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+      <c r="C49" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="C48" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>95</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D49" s="10" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>101</v>
-      </c>
-      <c r="C50" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+      <c r="C50" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>100</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>113</v>
+      </c>
+      <c r="C53" s="2" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>97</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C54" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="D54" s="10"/>
+      <c r="F54" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>116</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>112</v>
-      </c>
-      <c r="C54" s="2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
+        <v>114</v>
+      </c>
+      <c r="C55" s="10" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="C55" s="10" t="s">
+    </row>
+    <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>155</v>
+      </c>
+      <c r="C57" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="D55" s="10" t="s">
+      <c r="D57" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="4" t="s">
+      <c r="D58" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F58" t="s">
         <v>119</v>
       </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="F56" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A57" s="9" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" s="3" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A58" s="9" t="s">
-        <v>150</v>
-      </c>
-      <c r="C58" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>151</v>
+        <v>147</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>148</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>154</v>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B61" s="10"/>
+      <c r="C61" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B62" s="10"/>
+      <c r="C62" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B63" s="10"/>
+      <c r="C63" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 612: Fixed logic in doc-gen script around regional HC tibco links that didnt need to
Fixed logic in doc-gen script around regional HC tibco links that didnt need to be QA-specific.  Setup prod 2019.05 values.

Related work items: #5411
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="174">
   <si>
     <t>Template</t>
   </si>
@@ -492,45 +492,18 @@
     <t>Full section for DB updates before the core/base release scripts run by DBA.</t>
   </si>
   <si>
-    <t>139 - 140 (Feb 27 - Mar 27)</t>
-  </si>
-  <si>
-    <t>RELEASE_2019_04</t>
-  </si>
-  <si>
-    <t>20190417.*</t>
-  </si>
-  <si>
-    <t>11.0</t>
-  </si>
-  <si>
     <t>11.0.0</t>
   </si>
   <si>
-    <t>04</t>
-  </si>
-  <si>
     <t>AzureReleaseList</t>
   </si>
   <si>
-    <t>10.9.0</t>
-  </si>
-  <si>
-    <t>CHG0037090</t>
-  </si>
-  <si>
     <t>ReleaseSeqNum</t>
   </si>
   <si>
     <t>__ReleaseYear__.__ReleaseSeqNum__</t>
   </si>
   <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Infor Item Listener&lt;br&gt;Icon Global Event Controller&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth API Controller&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
-  </si>
-  <si>
-    <t>PublishReceivedOrderService</t>
-  </si>
-  <si>
     <t>05</t>
   </si>
   <si>
@@ -571,6 +544,27 @@
   </si>
   <si>
     <t>Flag 0 or 1 to indicate if QAF links should be generated for HoneyCrisp tibco apps</t>
+  </si>
+  <si>
+    <t>CHG0037407</t>
+  </si>
+  <si>
+    <t>141 - 142 (Mar 27 - Apr 24)</t>
+  </si>
+  <si>
+    <t>20190501.*</t>
+  </si>
+  <si>
+    <t>SO,SW</t>
+  </si>
+  <si>
+    <t>Deploy IRMA Suite Web App update and disable Promo Planner and Store Order Guide web apps.</t>
+  </si>
+  <si>
+    <t>IRMA Suite</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Icon Dashboard&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
   </si>
 </sst>
 </file>
@@ -965,9 +959,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A58" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1004,7 +998,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1026,7 +1020,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,11 +1064,11 @@
     </row>
     <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1083,7 +1077,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="9" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1222,7 +1216,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>123</v>
@@ -1236,7 +1230,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,7 +1285,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1299,7 +1293,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,7 +1438,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>124</v>
@@ -1452,22 +1446,22 @@
     </row>
     <row r="47" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -1487,7 +1481,7 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -1549,10 +1543,10 @@
     </row>
     <row r="57" spans="1:6" ht="330" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1619,9 +1613,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A49" sqref="A49"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1656,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>157</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,7 +1678,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>149</v>
+        <v>168</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1714,7 +1708,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>43517</v>
+        <v>43608</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,11 +1721,11 @@
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1740,7 +1734,7 @@
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="9" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1846,7 +1840,7 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,7 +1851,7 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,7 +1900,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1914,7 +1908,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2108,22 +2102,22 @@
     </row>
     <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -2143,7 +2137,7 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -2181,7 +2175,7 @@
         <v>98</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
       <c r="D54" s="10"/>
       <c r="F54" s="10" t="s">
@@ -2193,7 +2187,7 @@
         <v>114</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>96</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2204,12 +2198,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="150" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>160</v>
+        <v>173</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
Merged PR 658: Release 2019.06 IRMA Client and IRMA DB updates, and release doc values
- Rel doc: 2019.06 QA values
- Increment IRMA Client and DB versions to 11.2 and archive post-deploys.
- Rel doc: Trimmed tibco app list in rel doc to only 2 Kit-Builder apps
- Rel doc: Added WFMUHS update

Related work items: #5416
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="180">
   <si>
     <t>Template</t>
   </si>
@@ -510,24 +510,12 @@
     <t>RELEASE_2019_05</t>
   </si>
   <si>
-    <t>20190405*</t>
-  </si>
-  <si>
     <t>11.1</t>
   </si>
   <si>
     <t>11.1.0</t>
   </si>
   <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;eWIC APL Listener&lt;br&gt;eWIC Error-Response Listener&lt;br&gt;Icon API Controller&lt;br&gt;Icon Dashboard&lt;br&gt;Icon Global Event Controller&lt;br&gt;Icon Item-Movement Listener&lt;br&gt;Icon Monitoring Service&lt;br&gt;Icon Nutrition Web API&lt;br&gt;Icon POS Push Controller&lt;br&gt;Icon R10 Listener&lt;br&gt;Icon TLog Controller&lt;br&gt;Icon VIM Locale Controller&lt;br&gt;Icon Web&lt;br&gt;Icon Web API&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth API Controller&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Price Controller&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
-  </si>
-  <si>
-    <t>CHG0037346</t>
-  </si>
-  <si>
-    <t>141 - 142</t>
-  </si>
-  <si>
     <t>ActivePriceArchiver,EmergencyPriceService,ErrorMessagesListener,ErrorMessagesMonitor,EslPriceListener,ExpiringTprService,InStockDequeueService,IrmaPriceListener,JobSchedulerService,LoggingService,MammothActivePriceService,MammothPriceListener,OnePlumPriceListener,PriceListenerMessageArchiver,PrimeAffinityListener,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,R10PriceService</t>
   </si>
   <si>
@@ -537,9 +525,6 @@
     <t>HcTibcoRegions</t>
   </si>
   <si>
-    <t>PN,SO,SW</t>
-  </si>
-  <si>
     <t>List of regions for which tibco deploy links should be generated for HoneyCrisp apps</t>
   </si>
   <si>
@@ -565,6 +550,39 @@
   </si>
   <si>
     <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Icon Dashboard&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>143 - 144 (Apr 24 - May 22)</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_06</t>
+  </si>
+  <si>
+    <t>2019052*</t>
+  </si>
+  <si>
+    <t>11.2</t>
+  </si>
+  <si>
+    <t>11.2.0</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Icon Dashboard&lt;br&gt;Icon Monitoring&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>CHG0037986</t>
+  </si>
+  <si>
+    <t>PublishInstructionListService,PublishKitsService</t>
+  </si>
+  <si>
+    <t>Deploy 2019.06 WFMUHS.xml update.</t>
+  </si>
+  <si>
+    <t>WFM Mobile Config File</t>
   </si>
 </sst>
 </file>
@@ -959,9 +977,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -998,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1019,8 +1037,8 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>160</v>
+      <c r="C4" s="9" t="s">
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="7">
-        <v>43587</v>
+        <v>43613</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1068,7 +1086,7 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>153</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1216,7 +1234,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>123</v>
@@ -1230,7 +1248,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1285,7 +1303,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1293,7 +1311,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>157</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,7 +1456,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>161</v>
+        <v>177</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>124</v>
@@ -1446,22 +1464,22 @@
     </row>
     <row r="47" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B47" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>164</v>
       </c>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -1508,7 +1526,7 @@
         <v>98</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>96</v>
+        <v>178</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>99</v>
@@ -1530,7 +1548,7 @@
         <v>114</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>96</v>
+        <v>179</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1541,12 +1559,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="330" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>150</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>158</v>
+      <c r="C57" s="10" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1613,9 +1631,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A55" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1674,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1678,7 +1696,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1851,7 +1869,7 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1900,7 +1918,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1908,7 +1926,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2094,7 +2112,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>128</v>
@@ -2102,22 +2120,22 @@
     </row>
     <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="B47" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>165</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>170</v>
       </c>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -2175,7 +2193,7 @@
         <v>98</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="D54" s="10"/>
       <c r="F54" s="10" t="s">
@@ -2187,7 +2205,7 @@
         <v>114</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2203,7 +2221,7 @@
         <v>150</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>120</v>

</xml_diff>

<commit_message>
Merged PR 713: 2019.06 prod rel-doc values
2019.06 prod rel-doc values

Related work items: #5427
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="176">
   <si>
     <t>Template</t>
   </si>
@@ -504,18 +504,6 @@
     <t>__ReleaseYear__.__ReleaseSeqNum__</t>
   </si>
   <si>
-    <t>05</t>
-  </si>
-  <si>
-    <t>RELEASE_2019_05</t>
-  </si>
-  <si>
-    <t>11.1</t>
-  </si>
-  <si>
-    <t>11.1.0</t>
-  </si>
-  <si>
     <t>ActivePriceArchiver,EmergencyPriceService,ErrorMessagesListener,ErrorMessagesMonitor,EslPriceListener,ExpiringTprService,InStockDequeueService,IrmaPriceListener,JobSchedulerService,LoggingService,MammothActivePriceService,MammothPriceListener,OnePlumPriceListener,PriceListenerMessageArchiver,PrimeAffinityListener,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,R10PriceService</t>
   </si>
   <si>
@@ -534,12 +522,6 @@
     <t>CHG0037407</t>
   </si>
   <si>
-    <t>141 - 142 (Mar 27 - Apr 24)</t>
-  </si>
-  <si>
-    <t>20190501.*</t>
-  </si>
-  <si>
     <t>SO,SW</t>
   </si>
   <si>
@@ -549,9 +531,6 @@
     <t>IRMA Suite</t>
   </si>
   <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Icon Dashboard&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
-  </si>
-  <si>
     <t>143 - 144 (Apr 24 - May 22)</t>
   </si>
   <si>
@@ -583,6 +562,15 @@
   </si>
   <si>
     <t>WFM Mobile Config File</t>
+  </si>
+  <si>
+    <t>141 - 144 (Mar 27 - May 22)</t>
+  </si>
+  <si>
+    <t>201905+</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Icon Monitoring&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
   </si>
 </sst>
 </file>
@@ -977,9 +965,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1016,7 +1004,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1038,7 +1026,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1086,7 +1074,7 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1234,7 +1222,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>123</v>
@@ -1248,7 +1236,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1303,7 +1291,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1311,7 +1299,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1456,7 +1444,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>124</v>
@@ -1464,22 +1452,22 @@
     </row>
     <row r="47" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -1526,7 +1514,7 @@
         <v>98</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>99</v>
@@ -1548,7 +1536,7 @@
         <v>114</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1564,7 +1552,7 @@
         <v>150</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1631,9 +1619,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1674,7 +1662,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1696,7 +1684,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1726,7 +1714,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="1">
-        <v>43608</v>
+        <v>43622</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1743,7 +1731,7 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1858,7 +1846,7 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>154</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1869,7 +1857,7 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1918,7 +1906,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1926,7 +1914,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2112,7 +2100,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="D46" s="10" t="s">
         <v>128</v>
@@ -2120,22 +2108,22 @@
     </row>
     <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="C47" s="9" t="s">
         <v>159</v>
-      </c>
-      <c r="B47" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>165</v>
       </c>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -2193,7 +2181,7 @@
         <v>98</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D54" s="10"/>
       <c r="F54" s="10" t="s">
@@ -2205,7 +2193,7 @@
         <v>114</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2216,16 +2204,17 @@
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>150</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>120</v>
       </c>
+      <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">

</xml_diff>

<commit_message>
Merged PR 769: 2019.07 Release Prep (version increment, DB-script archive)
- - Rel-doc values for 2019.07 QA.
- Archived IRMA pre- and post-deploys.
- Updated IRMA DB and Client version files.
- Archived Icon-DB post-deploy scripts.

Related work items: #5434
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="177">
   <si>
     <t>Template</t>
   </si>
@@ -313,9 +313,6 @@
   </si>
   <si>
     <t>MammothManualDeploy</t>
-  </si>
-  <si>
-    <t>Manually deploy updated apps to Perf instances on Mammoth job server</t>
   </si>
   <si>
     <t>*NONE*</t>
@@ -531,39 +528,21 @@
     <t>IRMA Suite</t>
   </si>
   <si>
-    <t>143 - 144 (Apr 24 - May 22)</t>
-  </si>
-  <si>
     <t>06</t>
   </si>
   <si>
     <t>RELEASE_2019_06</t>
   </si>
   <si>
-    <t>2019052*</t>
-  </si>
-  <si>
     <t>11.2</t>
   </si>
   <si>
     <t>11.2.0</t>
   </si>
   <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Icon Dashboard&lt;br&gt;Icon Monitoring&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
-  </si>
-  <si>
-    <t>CHG0037986</t>
-  </si>
-  <si>
     <t>PublishInstructionListService,PublishKitsService</t>
   </si>
   <si>
-    <t>Deploy 2019.06 WFMUHS.xml update.</t>
-  </si>
-  <si>
-    <t>WFM Mobile Config File</t>
-  </si>
-  <si>
     <t>141 - 144 (Mar 27 - May 22)</t>
   </si>
   <si>
@@ -571,6 +550,30 @@
   </si>
   <si>
     <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Icon Monitoring&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>145 - 146 (May 22 - June 19)</t>
+  </si>
+  <si>
+    <t>CHG0038544</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_07</t>
+  </si>
+  <si>
+    <t>2019062*</t>
+  </si>
+  <si>
+    <t>11.3</t>
+  </si>
+  <si>
+    <t>11.3.0</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Infor Hierarchy-Class Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Icon Global Event Controller&lt;br&gt;Icon Web&lt;br&gt;Icon Dashboard&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Item-Locale Controller</t>
   </si>
 </sst>
 </file>
@@ -965,9 +968,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,13 +984,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1004,7 +1007,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1026,7 +1029,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>162</v>
+        <v>169</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1056,12 +1059,12 @@
         <v>8</v>
       </c>
       <c r="C7" s="7">
-        <v>43613</v>
+        <v>43641</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" s="10"/>
       <c r="C8" s="9">
@@ -1070,20 +1073,20 @@
     </row>
     <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>163</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1174,10 +1177,10 @@
     </row>
     <row r="21" spans="1:4" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -1196,7 +1199,7 @@
     </row>
     <row r="23" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>90</v>
@@ -1208,7 +1211,7 @@
         <v>92</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>93</v>
@@ -1222,10 +1225,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1236,7 +1239,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>165</v>
+        <v>173</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,7 +1261,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1269,7 +1272,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1291,7 +1294,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1299,7 +1302,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>167</v>
+        <v>175</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1444,30 +1447,30 @@
         <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="D46" s="12" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>156</v>
-      </c>
       <c r="C47" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -1487,20 +1490,20 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>95</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>61</v>
@@ -1508,105 +1511,105 @@
     </row>
     <row r="53" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" t="s">
         <v>97</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="D53" s="2" t="s">
         <v>98</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>171</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="F54" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>172</v>
+        <v>61</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>148</v>
-      </c>
       <c r="C59" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C63" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -1619,8 +1622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
     </sheetView>
   </sheetViews>
@@ -1636,13 +1639,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1651,7 +1654,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1662,7 +1665,7 @@
         <v>4</v>
       </c>
       <c r="C2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,7 +1687,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1703,7 +1706,7 @@
         <v>83</v>
       </c>
       <c r="C6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1719,7 +1722,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8">
         <v>2019</v>
@@ -1727,20 +1730,20 @@
     </row>
     <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="10"/>
       <c r="C10" s="9" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1834,7 +1837,7 @@
         <v>92</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D21" s="2"/>
     </row>
@@ -1846,7 +1849,7 @@
         <v>11</v>
       </c>
       <c r="C22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1857,7 +1860,7 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1887,7 +1890,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1906,7 +1909,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1914,7 +1917,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1966,11 +1969,11 @@
     </row>
     <row r="34" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B34" s="10"/>
       <c r="C34" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="105" x14ac:dyDescent="0.25">
@@ -1981,7 +1984,7 @@
         <v>26</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>89</v>
@@ -1990,19 +1993,19 @@
         <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B36" s="10"/>
       <c r="C36" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2018,7 +2021,7 @@
         <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2026,7 +2029,7 @@
         <v>67</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2034,7 +2037,7 @@
         <v>70</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2056,7 +2059,7 @@
         <v>75</v>
       </c>
       <c r="C42" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -2067,7 +2070,7 @@
         <v>75</v>
       </c>
       <c r="C43" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -2078,7 +2081,7 @@
         <v>75</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -2089,10 +2092,10 @@
         <v>75</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
@@ -2100,30 +2103,30 @@
         <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="9" t="s">
+        <v>154</v>
+      </c>
+      <c r="B47" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>156</v>
-      </c>
       <c r="C47" s="9" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D47" s="12"/>
     </row>
     <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="9" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C48" s="9">
         <v>0</v>
@@ -2143,7 +2146,7 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -2151,15 +2154,15 @@
         <v>94</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>61</v>
@@ -2167,117 +2170,117 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>96</v>
+      </c>
+      <c r="B54" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="B54" s="10" t="s">
-        <v>98</v>
-      </c>
       <c r="C54" s="10" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D54" s="10"/>
       <c r="F54" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56" s="2" t="s">
         <v>110</v>
-      </c>
-      <c r="C56" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="165" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F57" s="10"/>
     </row>
     <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B58" s="5"/>
       <c r="C58" s="5" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F58" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B59" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="B59" s="10" t="s">
-        <v>148</v>
-      </c>
       <c r="C59" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C60" s="3" t="s">
         <v>144</v>
-      </c>
-      <c r="B60" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="C60" s="3" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B61" s="10"/>
       <c r="C61" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B63" s="10"/>
       <c r="C63" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 932: 2019.08 Release Prep: rel doc, DB scripts
- QA rel doc.  Updated gen script to create the 4 sub-instances for in-stock tibco app.
- Archived 2019.07 release IRMA DB post-deploys.  Added PBI21615 pop-data to IRMA DB proj.  Updated IRMA DB version script.
- Archived 2019.07 release Mammoth-DB post-deploy.
- Section 12 Post Deploy: Added restart apps for dependent teams.
- QA rel doc: e-inv deploy

Related work items: #5467
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="180">
   <si>
     <t>Template</t>
   </si>
@@ -540,9 +540,6 @@
     <t>11.2.0</t>
   </si>
   <si>
-    <t>PublishInstructionListService,PublishKitsService</t>
-  </si>
-  <si>
     <t>141 - 144 (Mar 27 - May 22)</t>
   </si>
   <si>
@@ -552,28 +549,40 @@
     <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Icon Monitoring&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
   </si>
   <si>
-    <t>145 - 146 (May 22 - June 19)</t>
-  </si>
-  <si>
-    <t>CHG0038544</t>
-  </si>
-  <si>
-    <t>07</t>
-  </si>
-  <si>
-    <t>RELEASE_2019_07</t>
-  </si>
-  <si>
-    <t>2019062*</t>
-  </si>
-  <si>
-    <t>11.3</t>
-  </si>
-  <si>
     <t>11.3.0</t>
   </si>
   <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Infor Hierarchy-Class Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Icon Global Event Controller&lt;br&gt;Icon Web&lt;br&gt;Icon Dashboard&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Item-Locale Controller</t>
+    <t>147 - 148 (June 19 - July 17)</t>
+  </si>
+  <si>
+    <t>08</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_08</t>
+  </si>
+  <si>
+    <t>2019072*</t>
+  </si>
+  <si>
+    <t>11.4</t>
+  </si>
+  <si>
+    <t>11.4.0</t>
+  </si>
+  <si>
+    <t>MammothPriceListener,PrimeAffinityListener,R10PriceService,PublishInstructionListService,PublishKitsService,InStockDequeueService,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,RePublishInventoryMessagesService</t>
+  </si>
+  <si>
+    <t>FL,PN,SO,SW</t>
+  </si>
+  <si>
+    <t>CHG0039245</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;(ESB Perf DNS) eWIC APL Listener&lt;br&gt;(ESB Perf DNS) eWIC Error Response Listener&lt;br&gt;(ESB Perf DNS) R10 Listener&lt;br&gt;Icon Dashboard&lt;br&gt;(ESB Perf DNS) Icon Item Movement Listener&lt;br&gt;Icon Nutrition Web API&lt;br&gt;(ESB Perf DNS) Icon Web&lt;br&gt;(ESB Perf DNS) Infor Hierarchy Class Listener&lt;br&gt;Infor Item Listener&lt;br&gt;(ESB Perf DNS) Infor New Item Service&lt;br&gt;(ESB Perf DNS) Mammoth API Controller&lt;br&gt;Mammoth Audit Service&lt;br&gt;(ESB Perf DNS) Mammoth Hierarchy Listener&lt;br&gt;(ESB Perf DNS) Mammoth Locale Listener&lt;br&gt;Mammoth Product Listener&lt;br&gt;(ESB Perf DNS) Mammoth PrimeAffinity Controller&lt;br&gt;Mammoth Web Support&lt;br&gt;(ESB Perf DNS) Mammoth Web API</t>
+  </si>
+  <si>
+    <t>Deploy update for E-Invoicing legacy app</t>
   </si>
 </sst>
 </file>
@@ -970,7 +979,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C61" sqref="C61"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1007,7 +1016,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1059,7 +1068,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="7">
-        <v>43641</v>
+        <v>43669</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1077,7 +1086,7 @@
       </c>
       <c r="B9" s="10"/>
       <c r="C9" s="11" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -1225,7 +1234,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D25" s="9" t="s">
         <v>122</v>
@@ -1239,7 +1248,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1294,7 +1303,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1302,7 +1311,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1447,7 +1456,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="D46" s="12" t="s">
         <v>123</v>
@@ -1461,7 +1470,7 @@
         <v>155</v>
       </c>
       <c r="C47" s="9" t="s">
-        <v>158</v>
+        <v>176</v>
       </c>
       <c r="D47" s="12"/>
     </row>
@@ -1490,7 +1499,7 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>164</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1517,7 +1526,7 @@
         <v>97</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>61</v>
+        <v>179</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>98</v>
@@ -1528,7 +1537,7 @@
         <v>112</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>61</v>
+        <v>124</v>
       </c>
       <c r="F54" t="s">
         <v>96</v>
@@ -1550,12 +1559,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="285" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>149</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1687,7 +1696,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1860,7 +1869,7 @@
         <v>47</v>
       </c>
       <c r="C23" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2212,7 +2221,7 @@
         <v>149</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D57" s="10" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Merged PR 1144: Release 2019.09 Setup: IRMA DB archive & version, client version, reldoc
- IRMA DB: Archived 2019.08 pop-data.  Incremented version.
- QA reldoc values
- Increment IRMA Client version to 11.5 for fast-track that came in.  Added client and DBs to azure-deploy list in reldoc.

Cherry picked from !1143

Related work items: #5481
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="177">
   <si>
     <t>Template</t>
   </si>
@@ -489,9 +489,6 @@
     <t>Full section for DB updates before the core/base release scripts run by DBA.</t>
   </si>
   <si>
-    <t>11.0.0</t>
-  </si>
-  <si>
     <t>AzureReleaseList</t>
   </si>
   <si>
@@ -501,9 +498,6 @@
     <t>__ReleaseYear__.__ReleaseSeqNum__</t>
   </si>
   <si>
-    <t>ActivePriceArchiver,EmergencyPriceService,ErrorMessagesListener,ErrorMessagesMonitor,EslPriceListener,ExpiringTprService,InStockDequeueService,IrmaPriceListener,JobSchedulerService,LoggingService,MammothActivePriceService,MammothPriceListener,OnePlumPriceListener,PriceListenerMessageArchiver,PrimeAffinityListener,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,R10PriceService</t>
-  </si>
-  <si>
     <t>HcGenerateQafLinks</t>
   </si>
   <si>
@@ -516,39 +510,12 @@
     <t>Flag 0 or 1 to indicate if QAF links should be generated for HoneyCrisp tibco apps</t>
   </si>
   <si>
-    <t>CHG0037407</t>
-  </si>
-  <si>
     <t>SO,SW</t>
   </si>
   <si>
-    <t>Deploy IRMA Suite Web App update and disable Promo Planner and Store Order Guide web apps.</t>
-  </si>
-  <si>
-    <t>IRMA Suite</t>
-  </si>
-  <si>
-    <t>06</t>
-  </si>
-  <si>
-    <t>RELEASE_2019_06</t>
-  </si>
-  <si>
-    <t>11.2</t>
-  </si>
-  <si>
-    <t>11.2.0</t>
-  </si>
-  <si>
-    <t>141 - 144 (Mar 27 - May 22)</t>
-  </si>
-  <si>
     <t>201905+</t>
   </si>
   <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Icon Monitoring&lt;br&gt;Icon Web&lt;br&gt;Infor Hierarchy Listener&lt;br&gt;Infor Item Listener&lt;br&gt;Infor New Item Service&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy-Class Listener&lt;br&gt;Mammoth Locale Listener&lt;br&gt;Mammoth Prime Affinity Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
-  </si>
-  <si>
     <t>11.3.0</t>
   </si>
   <si>
@@ -561,28 +528,52 @@
     <t>RELEASE_2019_08</t>
   </si>
   <si>
-    <t>2019072*</t>
-  </si>
-  <si>
     <t>11.4</t>
   </si>
   <si>
     <t>11.4.0</t>
   </si>
   <si>
-    <t>MammothPriceListener,PrimeAffinityListener,R10PriceService,PublishInstructionListService,PublishKitsService,InStockDequeueService,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,RePublishInventoryMessagesService</t>
-  </si>
-  <si>
     <t>FL,PN,SO,SW</t>
   </si>
   <si>
-    <t>CHG0039245</t>
-  </si>
-  <si>
-    <t>&lt;hr&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;(ESB Perf DNS) eWIC APL Listener&lt;br&gt;(ESB Perf DNS) eWIC Error Response Listener&lt;br&gt;(ESB Perf DNS) R10 Listener&lt;br&gt;Icon Dashboard&lt;br&gt;(ESB Perf DNS) Icon Item Movement Listener&lt;br&gt;Icon Nutrition Web API&lt;br&gt;(ESB Perf DNS) Icon Web&lt;br&gt;(ESB Perf DNS) Infor Hierarchy Class Listener&lt;br&gt;Infor Item Listener&lt;br&gt;(ESB Perf DNS) Infor New Item Service&lt;br&gt;(ESB Perf DNS) Mammoth API Controller&lt;br&gt;Mammoth Audit Service&lt;br&gt;(ESB Perf DNS) Mammoth Hierarchy Listener&lt;br&gt;(ESB Perf DNS) Mammoth Locale Listener&lt;br&gt;Mammoth Product Listener&lt;br&gt;(ESB Perf DNS) Mammoth PrimeAffinity Controller&lt;br&gt;Mammoth Web Support&lt;br&gt;(ESB Perf DNS) Mammoth Web API</t>
-  </si>
-  <si>
     <t>Deploy update for E-Invoicing legacy app</t>
+  </si>
+  <si>
+    <t>CHG0039484</t>
+  </si>
+  <si>
+    <t>PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;Icon API Controller&lt;br&gt;Icon Nutrition Web API&lt;br&gt;Infor Item Listener&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Product Listener</t>
+  </si>
+  <si>
+    <t>CHG0039922</t>
+  </si>
+  <si>
+    <t>149 - 150 (July 17 - August 14)</t>
+  </si>
+  <si>
+    <t>09</t>
+  </si>
+  <si>
+    <t>20190818*</t>
+  </si>
+  <si>
+    <t>RELEASE_2019_09</t>
+  </si>
+  <si>
+    <t>11.5</t>
+  </si>
+  <si>
+    <t>11.5.0</t>
+  </si>
+  <si>
+    <t>EmergencyPriceService,ErrorMessagesMonitor,JobSchedulerService,MammothActivePriceService</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Icon Global Event Controller&lt;br&gt;Icon Web&lt;br&gt;Icon Dashboard&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
   </si>
 </sst>
 </file>
@@ -592,7 +583,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -606,6 +597,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -636,7 +633,6 @@
   </cellStyleXfs>
   <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -661,6 +657,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -979,7 +978,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,8 +1014,8 @@
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>177</v>
+      <c r="C2" s="5" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1026,7 +1025,7 @@
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1037,7 +1036,7 @@
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
+      <c r="C4" s="8" t="s">
         <v>169</v>
       </c>
     </row>
@@ -1048,7 +1047,7 @@
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1056,7 +1055,7 @@
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>58</v>
       </c>
     </row>
@@ -1067,42 +1066,42 @@
       <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="7">
-        <v>43669</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
+      <c r="C7" s="6">
+        <v>43697</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="10"/>
-      <c r="C8" s="9">
+      <c r="B8" s="9"/>
+      <c r="C8" s="8">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1110,7 +1109,7 @@
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1118,7 +1117,7 @@
       <c r="A13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1126,7 +1125,7 @@
       <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1134,7 +1133,7 @@
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1142,7 +1141,7 @@
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1150,7 +1149,7 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1158,7 +1157,7 @@
       <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1184,11 +1183,11 @@
         <v>61</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="1:4" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="C21" s="3" t="s">
+      <c r="C21" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1199,30 +1198,30 @@
       <c r="B22" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="C23" s="10" t="s">
+      <c r="C23" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="D23" s="10"/>
+      <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>92</v>
       </c>
-      <c r="C24" s="10" t="s">
+      <c r="C24" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="D24" s="10" t="s">
+      <c r="D24" s="9" t="s">
         <v>93</v>
       </c>
     </row>
@@ -1233,10 +1232,10 @@
       <c r="B25" t="s">
         <v>11</v>
       </c>
-      <c r="C25" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="D25" s="9" t="s">
+      <c r="C25" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="D25" s="8" t="s">
         <v>122</v>
       </c>
     </row>
@@ -1247,8 +1246,8 @@
       <c r="B26" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="11" t="s">
-        <v>172</v>
+      <c r="C26" s="10" t="s">
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1258,7 +1257,7 @@
       <c r="B27" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1269,7 +1268,7 @@
       <c r="B28" t="s">
         <v>13</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1280,7 +1279,7 @@
       <c r="B29" t="s">
         <v>48</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1291,7 +1290,7 @@
       <c r="B30" t="s">
         <v>14</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="C30" s="10" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1302,7 +1301,7 @@
       <c r="B31" t="s">
         <v>15</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="C31" s="10" t="s">
         <v>173</v>
       </c>
     </row>
@@ -1310,7 +1309,7 @@
       <c r="A32" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>174</v>
       </c>
     </row>
@@ -1321,7 +1320,7 @@
       <c r="B33" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="13" t="str">
+      <c r="C33" s="12" t="str">
         <f>C10</f>
         <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
@@ -1333,7 +1332,7 @@
       <c r="B34" t="s">
         <v>17</v>
       </c>
-      <c r="C34" s="13" t="str">
+      <c r="C34" s="12" t="str">
         <f>C10</f>
         <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
@@ -1345,7 +1344,7 @@
       <c r="B35" t="s">
         <v>18</v>
       </c>
-      <c r="C35" s="13" t="str">
+      <c r="C35" s="12" t="str">
         <f>C10</f>
         <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
@@ -1444,10 +1443,10 @@
       <c r="B45" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="C45" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1455,42 +1454,42 @@
       <c r="A46" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="11" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="47" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+    <row r="47" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>176</v>
-      </c>
-      <c r="D47" s="12"/>
-    </row>
-    <row r="48" spans="1:4" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C48" s="9">
+      <c r="C48" s="8">
         <v>0</v>
       </c>
-      <c r="D48" s="12"/>
+      <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="1" t="s">
         <v>88</v>
       </c>
     </row>
@@ -1499,14 +1498,14 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="1" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1514,7 +1513,7 @@
       <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1525,10 +1524,10 @@
       <c r="B53" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="D53" s="2" t="s">
+      <c r="C53" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1536,7 +1535,7 @@
       <c r="A54" t="s">
         <v>112</v>
       </c>
-      <c r="C54" s="2" t="s">
+      <c r="C54" s="1" t="s">
         <v>124</v>
       </c>
       <c r="F54" t="s">
@@ -1547,7 +1546,7 @@
       <c r="A55" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="2" t="s">
+      <c r="C55" s="1" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1555,45 +1554,45 @@
       <c r="A56" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="285" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" s="10" t="s">
-        <v>178</v>
+        <v>148</v>
+      </c>
+      <c r="C57" s="9" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C58" s="5" t="s">
+      <c r="C58" s="4" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="59" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="60" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>144</v>
       </c>
     </row>
@@ -1601,23 +1600,23 @@
       <c r="A61" t="s">
         <v>134</v>
       </c>
-      <c r="C61" s="3" t="s">
+      <c r="C61" s="2" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+      <c r="A62" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="C62" s="3" t="s">
+      <c r="C62" s="2" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+      <c r="A63" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="C63" s="3" t="s">
+      <c r="C63" s="2" t="s">
         <v>139</v>
       </c>
     </row>
@@ -1633,13 +1632,13 @@
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F57" sqref="F57"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="38.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.140625" style="10" customWidth="1"/>
+    <col min="2" max="2" width="58.140625" style="9" customWidth="1"/>
     <col min="3" max="3" width="41.85546875" customWidth="1"/>
     <col min="4" max="4" width="32.28515625" customWidth="1"/>
     <col min="5" max="5" width="16.5703125" customWidth="1"/>
@@ -1647,10 +1646,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="8" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
@@ -1670,21 +1669,21 @@
       <c r="A2" t="s">
         <v>40</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>157</v>
+      <c r="C2" s="8" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>57</v>
       </c>
     </row>
@@ -1692,21 +1691,21 @@
       <c r="A4" t="s">
         <v>30</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>165</v>
+      <c r="C4" s="8" t="s">
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="8" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1714,7 +1713,7 @@
       <c r="A6" t="s">
         <v>83</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="8" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1722,60 +1721,60 @@
       <c r="A7" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="1">
-        <v>43622</v>
+      <c r="C7" s="6">
+        <v>43685</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>101</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="8">
         <v>2019</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="B10" s="10"/>
-      <c r="C10" s="9" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
-      <c r="C11" t="s">
-        <v>55</v>
+      <c r="C11" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>35</v>
       </c>
-      <c r="C12" t="s">
-        <v>55</v>
+      <c r="C12" s="8" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1783,7 +1782,7 @@
       <c r="A14" t="s">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1791,7 +1790,7 @@
       <c r="A15" t="s">
         <v>37</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1799,7 +1798,7 @@
       <c r="A16" t="s">
         <v>38</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1807,7 +1806,7 @@
       <c r="A17" t="s">
         <v>39</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1815,7 +1814,7 @@
       <c r="A18" t="s">
         <v>33</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="8" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1823,10 +1822,10 @@
       <c r="A19" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1834,10 +1833,10 @@
       <c r="A20" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1845,49 +1844,50 @@
       <c r="A21" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="D21" s="2"/>
+      <c r="D21" s="1"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="B22" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C22" t="s">
-        <v>162</v>
+      <c r="C22" s="8" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>50</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="C23" t="s">
-        <v>166</v>
+      <c r="C23" s="8" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>51</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="B24" s="9" t="s">
         <v>12</v>
       </c>
+      <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="B25" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="8" t="s">
         <v>61</v>
       </c>
     </row>
@@ -1895,10 +1895,10 @@
       <c r="A26" t="s">
         <v>49</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="B26" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C26" s="9" t="s">
+      <c r="C26" s="8" t="s">
         <v>141</v>
       </c>
     </row>
@@ -1906,37 +1906,38 @@
       <c r="A27" t="s">
         <v>54</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="B27" s="9" t="s">
         <v>14</v>
       </c>
+      <c r="C27" s="8"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>43</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="B28" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="11" t="s">
-        <v>163</v>
+      <c r="C28" s="10" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>71</v>
       </c>
-      <c r="C29" s="11" t="s">
-        <v>164</v>
+      <c r="C29" s="10" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>44</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C30" s="13" t="str">
+      <c r="C30" s="12" t="str">
         <f>C10</f>
         <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
@@ -1945,10 +1946,10 @@
       <c r="A31" t="s">
         <v>45</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="B31" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C31" s="13" t="str">
+      <c r="C31" s="12" t="str">
         <f>C10</f>
         <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
@@ -1957,10 +1958,10 @@
       <c r="A32" t="s">
         <v>46</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="B32" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C32" s="13" t="str">
+      <c r="C32" s="12" t="str">
         <f>C10</f>
         <v>__ReleaseYear__.__ReleaseSeqNum__</v>
       </c>
@@ -1969,19 +1970,19 @@
       <c r="A33" t="s">
         <v>62</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="B33" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="8" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
         <v>133</v>
       </c>
-      <c r="B34" s="10"/>
-      <c r="C34" s="3" t="s">
+      <c r="B34" s="9"/>
+      <c r="C34" s="2" t="s">
         <v>130</v>
       </c>
     </row>
@@ -1989,31 +1990,31 @@
       <c r="A35" t="s">
         <v>91</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="3" t="s">
+      <c r="C35" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D35" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="E35" s="1" t="s">
         <v>90</v>
       </c>
       <c r="F35" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="36" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
+    <row r="36" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B36" s="10"/>
-      <c r="C36" s="3" t="s">
+      <c r="B36" s="9"/>
+      <c r="C36" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="D36" s="3" t="s">
+      <c r="D36" s="2" t="s">
         <v>128</v>
       </c>
     </row>
@@ -2021,7 +2022,7 @@
       <c r="A37" t="s">
         <v>63</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="8" t="s">
         <v>64</v>
       </c>
     </row>
@@ -2029,7 +2030,7 @@
       <c r="A38" t="s">
         <v>65</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="8" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2037,7 +2038,7 @@
       <c r="A39" t="s">
         <v>67</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="8" t="s">
         <v>105</v>
       </c>
     </row>
@@ -2045,7 +2046,7 @@
       <c r="A40" t="s">
         <v>70</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="C40" s="9" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2053,10 +2054,10 @@
       <c r="A41" t="s">
         <v>72</v>
       </c>
-      <c r="B41" s="10" t="s">
+      <c r="B41" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="8" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2064,10 +2065,10 @@
       <c r="A42" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="10" t="s">
+      <c r="B42" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="8" t="s">
         <v>107</v>
       </c>
     </row>
@@ -2075,10 +2076,10 @@
       <c r="A43" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="10" t="s">
+      <c r="B43" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="8" t="s">
         <v>108</v>
       </c>
     </row>
@@ -2086,10 +2087,10 @@
       <c r="A44" t="s">
         <v>78</v>
       </c>
-      <c r="B44" s="10" t="s">
+      <c r="B44" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="8" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2097,13 +2098,13 @@
       <c r="A45" t="s">
         <v>79</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="B45" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="C45" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D45" s="1" t="s">
         <v>114</v>
       </c>
     </row>
@@ -2111,42 +2112,42 @@
       <c r="A46" t="s">
         <v>85</v>
       </c>
-      <c r="C46" s="9" t="s">
+      <c r="C46" s="8" t="s">
+        <v>166</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="D46" s="10" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="9" t="s">
+      <c r="B47" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>155</v>
+      </c>
+      <c r="D47" s="11"/>
+    </row>
+    <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B47" s="9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C47" s="9" t="s">
-        <v>158</v>
-      </c>
-      <c r="D47" s="12"/>
-    </row>
-    <row r="48" spans="1:6" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="9" t="s">
-        <v>153</v>
-      </c>
-      <c r="B48" s="9" t="s">
-        <v>156</v>
-      </c>
-      <c r="C48" s="9">
+      <c r="C48" s="8">
         <v>0</v>
       </c>
-      <c r="D48" s="12"/>
+      <c r="D48" s="11"/>
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
-      <c r="C49" s="2" t="s">
+      <c r="C49" s="9" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2154,18 +2155,18 @@
       <c r="A50" t="s">
         <v>87</v>
       </c>
-      <c r="C50" t="s">
-        <v>148</v>
+      <c r="C50" s="8" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="2" t="s">
+      <c r="C51" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="9" t="s">
         <v>111</v>
       </c>
     </row>
@@ -2173,7 +2174,7 @@
       <c r="A52" t="s">
         <v>99</v>
       </c>
-      <c r="C52" s="2" t="s">
+      <c r="C52" s="9" t="s">
         <v>61</v>
       </c>
     </row>
@@ -2181,7 +2182,7 @@
       <c r="A53" t="s">
         <v>112</v>
       </c>
-      <c r="C53" s="2" t="s">
+      <c r="C53" s="9" t="s">
         <v>124</v>
       </c>
     </row>
@@ -2189,14 +2190,14 @@
       <c r="A54" t="s">
         <v>96</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="B54" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="D54" s="10"/>
-      <c r="F54" s="10" t="s">
+      <c r="C54" s="9" t="s">
+        <v>164</v>
+      </c>
+      <c r="D54" s="9"/>
+      <c r="F54" s="9" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2204,91 +2205,91 @@
       <c r="A55" t="s">
         <v>113</v>
       </c>
-      <c r="C55" s="10" t="s">
-        <v>160</v>
+      <c r="C55" s="9" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="2" t="s">
+      <c r="C56" s="9" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="165" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="66" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>149</v>
-      </c>
-      <c r="C57" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="C57" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="9" t="s">
         <v>119</v>
       </c>
-      <c r="F57" s="10"/>
+      <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="A58" s="4" t="s">
+      <c r="A58" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B58" s="5"/>
-      <c r="C58" s="5" t="s">
+      <c r="B58" s="4"/>
+      <c r="C58" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="4" t="s">
         <v>120</v>
       </c>
       <c r="F58" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="9" t="s">
+    <row r="59" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="B59" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="C59" s="3" t="s">
+      <c r="C59" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:6" s="9" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="9" t="s">
+    <row r="60" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B60" s="9" t="s">
         <v>145</v>
       </c>
-      <c r="C60" s="3" t="s">
+      <c r="C60" s="2" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="61" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A61" s="9" t="s">
+    <row r="61" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
         <v>134</v>
       </c>
-      <c r="B61" s="10"/>
-      <c r="C61" s="3" t="s">
+      <c r="B61" s="9"/>
+      <c r="C61" s="2" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="62" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A62" s="9" t="s">
+    <row r="62" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
         <v>135</v>
       </c>
-      <c r="B62" s="10"/>
-      <c r="C62" s="3" t="s">
+      <c r="B62" s="9"/>
+      <c r="C62" s="2" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="63" spans="1:6" s="9" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="9" t="s">
+    <row r="63" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="B63" s="10"/>
-      <c r="C63" s="3" t="s">
+      <c r="B63" s="9"/>
+      <c r="C63" s="2" t="s">
         <v>139</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Merged PR 1219: RelDoc changes for PRD Release 2019.09
RelDoc changes for PRD Release 2019.09

Related work items: #5488
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\scad\DevOps\Release Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arturo.rivas\source\repos\SCAD\DevOps\Release Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="170">
   <si>
     <t>Template</t>
   </si>
@@ -510,45 +510,12 @@
     <t>Flag 0 or 1 to indicate if QAF links should be generated for HoneyCrisp tibco apps</t>
   </si>
   <si>
-    <t>SO,SW</t>
-  </si>
-  <si>
-    <t>201905+</t>
-  </si>
-  <si>
-    <t>11.3.0</t>
-  </si>
-  <si>
-    <t>147 - 148 (June 19 - July 17)</t>
-  </si>
-  <si>
-    <t>08</t>
-  </si>
-  <si>
-    <t>RELEASE_2019_08</t>
-  </si>
-  <si>
-    <t>11.4</t>
-  </si>
-  <si>
     <t>11.4.0</t>
   </si>
   <si>
     <t>FL,PN,SO,SW</t>
   </si>
   <si>
-    <t>Deploy update for E-Invoicing legacy app</t>
-  </si>
-  <si>
-    <t>CHG0039484</t>
-  </si>
-  <si>
-    <t>PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService</t>
-  </si>
-  <si>
-    <t>&lt;hr&gt;Icon API Controller&lt;br&gt;Icon Nutrition Web API&lt;br&gt;Infor Item Listener&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Product Listener</t>
-  </si>
-  <si>
     <t>CHG0039922</t>
   </si>
   <si>
@@ -574,6 +541,18 @@
   </si>
   <si>
     <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Icon Global Event Controller&lt;br&gt;Icon Web&lt;br&gt;Icon Dashboard&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>Arturo Rivas</t>
+  </si>
+  <si>
+    <t>CHG0040169</t>
+  </si>
+  <si>
+    <t>EmergencyPriceService,ErrorMessagesMonitor,JobSchedulerService</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Icon Global Event Controller&lt;br&gt;Icon Web&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API&lt;br&gt;Mammoth Web Support</t>
   </si>
 </sst>
 </file>
@@ -976,9 +955,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1015,7 +994,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1037,7 +1016,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,7 +1064,7 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1233,7 +1212,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>122</v>
@@ -1247,7 +1226,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1302,7 +1281,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1310,7 +1289,7 @@
         <v>71</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1455,7 +1434,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>123</v>
@@ -1469,7 +1448,7 @@
         <v>153</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>163</v>
+        <v>156</v>
       </c>
       <c r="D47" s="11"/>
     </row>
@@ -1498,7 +1477,7 @@
         <v>87</v>
       </c>
       <c r="C50" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1563,7 +1542,7 @@
         <v>148</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1630,9 +1609,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A50" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1673,7 +1652,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1684,7 +1663,7 @@
         <v>5</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>57</v>
+        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1725,7 +1704,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="6">
-        <v>43685</v>
+        <v>43713</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1759,7 +1738,7 @@
         <v>34</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,7 +1746,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1775,7 +1754,7 @@
         <v>42</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1857,7 +1836,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1868,7 +1847,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>156</v>
+        <v>160</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1919,7 +1898,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1927,7 +1906,7 @@
         <v>71</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2113,7 +2092,7 @@
         <v>85</v>
       </c>
       <c r="C46" s="8" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>127</v>
@@ -2127,7 +2106,7 @@
         <v>153</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D47" s="11"/>
     </row>
@@ -2156,7 +2135,7 @@
         <v>87</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -2194,7 +2173,7 @@
         <v>97</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="D54" s="9"/>
       <c r="F54" s="9" t="s">
@@ -2217,12 +2196,12 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="66" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="99" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>148</v>
       </c>
       <c r="C57" s="13" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>119</v>

</xml_diff>

<commit_message>
Merged PR 2628: 2020.01 release doc
- Release doc.
- Added IRMA QA1 ref for target DB so updates are applied there as well.

Related work items: #5531
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="175">
   <si>
     <t>Template</t>
   </si>
@@ -224,9 +224,6 @@
   </si>
   <si>
     <t>IrmaDbServer</t>
-  </si>
-  <si>
-    <t>IDQ-xx\xxQ</t>
   </si>
   <si>
     <t>IconDbServer</t>
@@ -513,12 +510,6 @@
     <t>FL,PN,SO,SW</t>
   </si>
   <si>
-    <t>153 - 154 (September 11 - October 9)</t>
-  </si>
-  <si>
-    <t>CHG0041277</t>
-  </si>
-  <si>
     <t>11</t>
   </si>
   <si>
@@ -537,13 +528,46 @@
     <t>11.6.0</t>
   </si>
   <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API</t>
-  </si>
-  <si>
-    <t>CHG0041301</t>
-  </si>
-  <si>
     <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API</t>
+  </si>
+  <si>
+    <t>CHG0042582</t>
+  </si>
+  <si>
+    <t>155 - 159 (October 9 - December 18)</t>
+  </si>
+  <si>
+    <t>CHG004????</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>RELEASE_2020_01</t>
+  </si>
+  <si>
+    <t>11.8</t>
+  </si>
+  <si>
+    <t>11.8.0</t>
+  </si>
+  <si>
+    <t>PublishTransferOrderService</t>
+  </si>
+  <si>
+    <t>FL,MA,MW,NA,NC,NE,PN,RM,SO,SP,SW</t>
+  </si>
+  <si>
+    <t>POS Push, PS Upload, PS Transfer Upload</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Mammoth DB (QA Only, not PERF)&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy Class Listener&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;POS Push Job&lt;li&gt;PeopleSoft Upload Job&lt;li&gt;PeopleSoft Transfer Upload Job&lt;li&gt;MILD SSIS Jobs&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>IDQ-xx\xxQ *AND* IRMA-xx-DB-QA</t>
   </si>
 </sst>
 </file>
@@ -937,9 +961,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,13 +977,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -976,7 +1000,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -998,7 +1022,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1014,7 +1038,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>58</v>
@@ -1028,34 +1052,34 @@
         <v>8</v>
       </c>
       <c r="C7" s="6">
-        <v>43753</v>
+        <v>43819</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="8">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1146,44 +1170,44 @@
     </row>
     <row r="21" spans="1:4" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>92</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>125</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1194,10 +1218,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>160</v>
+        <v>166</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1208,7 +1232,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,7 +1254,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1241,7 +1265,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1263,15 +1287,15 @@
         <v>15</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>161</v>
+        <v>167</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1334,112 +1358,112 @@
         <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>174</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
         <v>67</v>
-      </c>
-      <c r="C39" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" t="s">
         <v>72</v>
-      </c>
-      <c r="B41" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" t="s">
         <v>74</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>75</v>
-      </c>
-      <c r="C42" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>144</v>
+        <v>169</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>153</v>
-      </c>
       <c r="C47" s="8" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C48" s="8">
         <v>0</v>
@@ -1448,31 +1472,31 @@
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>61</v>
@@ -1480,105 +1504,105 @@
     </row>
     <row r="53" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>95</v>
+      </c>
+      <c r="B53" t="s">
         <v>96</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>144</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F54" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>61</v>
+        <v>171</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>164</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B59" s="9" t="s">
-        <v>147</v>
-      </c>
       <c r="C59" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1591,9 +1615,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1608,13 +1632,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1623,7 +1647,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1634,7 +1658,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1656,7 +1680,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>156</v>
+        <v>163</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1667,15 +1691,15 @@
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1691,7 +1715,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" s="8">
         <v>2019</v>
@@ -1699,20 +1723,20 @@
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="8" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1803,10 +1827,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1818,7 +1842,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1829,7 +1853,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1860,7 +1884,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1880,15 +1904,15 @@
         <v>15</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1940,43 +1964,43 @@
     </row>
     <row r="34" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>90</v>
-      </c>
       <c r="F35" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1992,112 +2016,112 @@
         <v>65</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>71</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>72</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>75</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>73</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>73</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>75</v>
-      </c>
       <c r="C42" s="8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B47" s="8" t="s">
-        <v>153</v>
-      </c>
       <c r="C47" s="8" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C48" s="8">
         <v>0</v>
@@ -2106,34 +2130,34 @@
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>93</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>95</v>
-      </c>
       <c r="D51" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>61</v>
@@ -2141,117 +2165,117 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>95</v>
+      </c>
+      <c r="B54" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>97</v>
-      </c>
       <c r="C54" s="9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D54" s="9"/>
       <c r="F54" s="9" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>108</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>109</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
+        <v>145</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>146</v>
       </c>
-      <c r="B59" s="9" t="s">
-        <v>147</v>
-      </c>
       <c r="C59" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
+        <v>142</v>
+      </c>
+      <c r="B60" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C60" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="B60" s="9" t="s">
-        <v>145</v>
-      </c>
-      <c r="C60" s="2" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 2788: RelDoc update for PRD Release 2020.1
For PRD Release on Jan 23rd

Related work items: #8185
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\scad\DevOps\Release Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arturo.rivas\source\repos\SCAD\DevOps\Release Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="171">
   <si>
     <t>Template</t>
   </si>
@@ -507,39 +507,18 @@
     <t>Flag 0 or 1 to indicate if QAF links should be generated for HoneyCrisp tibco apps</t>
   </si>
   <si>
-    <t>FL,PN,SO,SW</t>
-  </si>
-  <si>
-    <t>11</t>
-  </si>
-  <si>
     <t>builds</t>
   </si>
   <si>
-    <t>RELEASE_2019_11</t>
-  </si>
-  <si>
-    <t>11.7</t>
-  </si>
-  <si>
     <t>11.7.0</t>
   </si>
   <si>
-    <t>11.6.0</t>
-  </si>
-  <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Web API</t>
-  </si>
-  <si>
     <t>CHG0042582</t>
   </si>
   <si>
     <t>155 - 159 (October 9 - December 18)</t>
   </si>
   <si>
-    <t>CHG004????</t>
-  </si>
-  <si>
     <t>01</t>
   </si>
   <si>
@@ -568,6 +547,15 @@
   </si>
   <si>
     <t>IDQ-xx\xxQ *AND* IRMA-xx-DB-QA</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>CHG0042994</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Mammoth DB&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy Class Listener&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Web Support</t>
   </si>
 </sst>
 </file>
@@ -961,8 +949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
@@ -1000,7 +988,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>162</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1022,7 +1010,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,7 +1058,7 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1218,7 +1206,7 @@
         <v>11</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>166</v>
+        <v>159</v>
       </c>
       <c r="D25" s="8" t="s">
         <v>121</v>
@@ -1232,7 +1220,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1287,7 +1275,7 @@
         <v>15</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>167</v>
+        <v>160</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -1295,7 +1283,7 @@
         <v>70</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>168</v>
+        <v>161</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1358,7 +1346,7 @@
         <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1440,7 +1428,7 @@
         <v>84</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>122</v>
@@ -1454,7 +1442,7 @@
         <v>152</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>170</v>
+        <v>163</v>
       </c>
       <c r="D47" s="11"/>
     </row>
@@ -1483,7 +1471,7 @@
         <v>86</v>
       </c>
       <c r="C50" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1510,7 +1498,7 @@
         <v>96</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D53" s="1" t="s">
         <v>97</v>
@@ -1532,7 +1520,7 @@
         <v>112</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1548,7 +1536,7 @@
         <v>147</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1615,9 +1603,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,7 +1646,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>164</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1680,7 +1668,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1710,7 +1698,7 @@
         <v>8</v>
       </c>
       <c r="C7" s="6">
-        <v>43762</v>
+        <v>43853</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1718,7 +1706,7 @@
         <v>100</v>
       </c>
       <c r="C8" s="8">
-        <v>2019</v>
+        <v>2020</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1727,7 +1715,7 @@
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>155</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
@@ -1776,7 +1764,7 @@
         <v>37</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1842,7 +1830,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1853,7 +1841,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1904,7 +1892,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1912,7 +1900,7 @@
         <v>70</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -2098,7 +2086,7 @@
         <v>84</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>94</v>
+        <v>162</v>
       </c>
       <c r="D46" s="9" t="s">
         <v>126</v>
@@ -2112,7 +2100,7 @@
         <v>152</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
       <c r="D47" s="11"/>
     </row>
@@ -2141,7 +2129,7 @@
         <v>86</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
@@ -2179,7 +2167,7 @@
         <v>96</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
       <c r="D54" s="9"/>
       <c r="F54" s="9" t="s">
@@ -2191,7 +2179,7 @@
         <v>112</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -2202,12 +2190,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>147</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>118</v>

</xml_diff>

<commit_message>
Merged PR 3918: Release 2020.03: QA reldoc, IRMA pre/post SQL archive, reldoc template IRMA app-settings, Prod WFMUHS
- QA rel doc
- Archiving IRMA Pre/Post deploy for 2020.03 release.
- Added rebuild of IRMA app-settings to sections 11 and 12
- Prod WFM-Mobile config update for IRMA Plugin v10.6.0.0 for 2020.03 release, all regions.

Related work items: #32631
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\arturo.rivas\source\repos\SCAD\DevOps\Release Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\tlux\dev\git\scad\DevOps\Release Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16740" windowHeight="6525"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="179">
   <si>
     <t>Template</t>
   </si>
@@ -229,9 +229,6 @@
     <t>IconDbServer</t>
   </si>
   <si>
-    <t>IDQ-Icon\SqlShared3Q</t>
-  </si>
-  <si>
     <t>Mammoth-DB01-QA\Mammoth</t>
   </si>
   <si>
@@ -263,12 +260,6 @@
   </si>
   <si>
     <t>TibcoServersAffected</t>
-  </si>
-  <si>
-    <t>VM-Icon-QA[1-4]</t>
-  </si>
-  <si>
-    <t>Mammoth-App01-QA</t>
   </si>
   <si>
     <t>QA: CERD1673, CERD1674 | QA-Perf: CERD1662, CERD1663, CERD1664, CERD1665</t>
@@ -513,15 +504,9 @@
     <t>11.7.0</t>
   </si>
   <si>
-    <t>CHG0042582</t>
-  </si>
-  <si>
     <t>155 - 159 (October 9 - December 18)</t>
   </si>
   <si>
-    <t>01</t>
-  </si>
-  <si>
     <t>RELEASE_2020_01</t>
   </si>
   <si>
@@ -540,9 +525,6 @@
     <t>POS Push, PS Upload, PS Transfer Upload</t>
   </si>
   <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Mammoth DB (QA Only, not PERF)&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy Class Listener&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Web Support</t>
-  </si>
-  <si>
     <t>&lt;ol&gt;&lt;li&gt;POS Push Job&lt;li&gt;PeopleSoft Upload Job&lt;li&gt;PeopleSoft Transfer Upload Job&lt;li&gt;MILD SSIS Jobs&lt;/ol&gt;</t>
   </si>
   <si>
@@ -556,6 +538,48 @@
   </si>
   <si>
     <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Mammoth DB&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy Class Listener&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Web Support</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>160 - 164 (December 18 - February 28)</t>
+  </si>
+  <si>
+    <t>CHG0044494</t>
+  </si>
+  <si>
+    <t>RELEASE_2020_03</t>
+  </si>
+  <si>
+    <t>11.9</t>
+  </si>
+  <si>
+    <t>11.9.0</t>
+  </si>
+  <si>
+    <t>Icon-DB-QA *AND* Icon-DB-QA-Perf</t>
+  </si>
+  <si>
+    <t>IrmaPriceListener,JobSchedulerService,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,PublishKitsService</t>
+  </si>
+  <si>
+    <t>11.8.1</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;IRMA Web Service&lt;li&gt;IRMA Mobile Plugin DLL&lt;li&gt;WFM Mobile Config File&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>IRMA Web Service, IRMA Mobile Plugin DLL, WFM Mobile Config File</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;All Icon Apps&lt;br&gt;Mammoth DB&lt;br&gt;All Mammoth Apps</t>
+  </si>
+  <si>
+    <t>IRMAQAJob[01-06], IRMAQAWeb[01-06]</t>
+  </si>
+  <si>
+    <t>IRMAQAJob[01-06]</t>
   </si>
 </sst>
 </file>
@@ -949,9 +973,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="A2:C63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,13 +989,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -988,7 +1012,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>156</v>
+        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1010,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1026,7 +1050,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>58</v>
@@ -1040,12 +1064,12 @@
         <v>8</v>
       </c>
       <c r="C7" s="6">
-        <v>43819</v>
+        <v>43893</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="8">
@@ -1054,20 +1078,20 @@
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>158</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1158,44 +1182,44 @@
     </row>
     <row r="21" spans="1:4" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D24" s="9" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1206,10 +1230,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1220,7 +1244,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1242,7 +1266,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1253,7 +1277,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1275,15 +1299,15 @@
         <v>15</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -1346,7 +1370,7 @@
         <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1354,104 +1378,104 @@
         <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" t="s">
         <v>71</v>
-      </c>
-      <c r="B41" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" t="s">
         <v>73</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>74</v>
-      </c>
-      <c r="C42" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>177</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>80</v>
+        <v>178</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
+        <v>77</v>
+      </c>
+      <c r="B45" t="s">
+        <v>73</v>
+      </c>
+      <c r="C45" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B45" t="s">
-        <v>74</v>
-      </c>
-      <c r="C45" s="7" t="s">
-        <v>81</v>
-      </c>
       <c r="D45" s="1" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>162</v>
+        <v>172</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="C48" s="8">
         <v>0</v>
@@ -1460,31 +1484,31 @@
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C50" t="s">
-        <v>155</v>
+        <v>173</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>61</v>
@@ -1492,105 +1516,105 @@
     </row>
     <row r="53" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B53" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>166</v>
+        <v>174</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="F54" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>164</v>
+        <v>175</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>130</v>
+      </c>
+      <c r="C61" s="2" t="s">
         <v>133</v>
-      </c>
-      <c r="C61" s="2" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C62" s="2" t="s">
         <v>134</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="C63" s="2" t="s">
         <v>135</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>138</v>
       </c>
     </row>
   </sheetData>
@@ -1603,9 +1627,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B61" sqref="B61"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,13 +1644,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1635,7 +1659,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1646,7 +1670,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1668,7 +1692,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1679,15 +1703,15 @@
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1703,7 +1727,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="C8" s="8">
         <v>2020</v>
@@ -1711,20 +1735,20 @@
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="8" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1815,10 +1839,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1830,7 +1854,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1841,7 +1865,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1872,7 +1896,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1892,15 +1916,15 @@
         <v>15</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1952,43 +1976,43 @@
     </row>
     <row r="34" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="2" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="F35" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2004,7 +2028,7 @@
         <v>65</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2012,104 +2036,104 @@
         <v>66</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>71</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>74</v>
-      </c>
       <c r="C42" s="8" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B43" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>150</v>
-      </c>
-      <c r="B48" s="8" t="s">
-        <v>153</v>
       </c>
       <c r="C48" s="8">
         <v>0</v>
@@ -2118,34 +2142,34 @@
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D51" s="9" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>61</v>
@@ -2153,117 +2177,117 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C54" s="9" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D54" s="9"/>
       <c r="F54" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C56" s="9" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F58" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="B60" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Merged PR 4682: 2020.06 release prep, archiving pre/post DB scripts
- 2020.06 reldoc
- Archiving 7 post-deploy scripts from 2020.05 release.
- Archiving already-applied Mammoth-DB pre- and post-deploy scripts.

Cherry picked from !4681

Related work items: #36294
</commit_message>
<xml_diff>
--- a/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
+++ b/DevOps/Release Documentation/Release Documentation Input Variables.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="331" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="179">
   <si>
     <t>Template</t>
   </si>
@@ -248,9 +248,6 @@
   </si>
   <si>
     <t>This should be dynamic</t>
-  </si>
-  <si>
-    <t>IRMAQAApp[1-4]</t>
   </si>
   <si>
     <t>IconServersAffected</t>
@@ -408,9 +405,6 @@
     <t>IRM</t>
   </si>
   <si>
-    <t>Mammoth-DB01-QA\Mammoth.Mammoth, QA-01-Mammoth02\Mammoth02.Mammoth</t>
-  </si>
-  <si>
     <t>MammothDbScriptLink</t>
   </si>
   <si>
@@ -540,46 +534,52 @@
     <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon API Controller&lt;br&gt;Mammoth DB&lt;br&gt;Mammoth Audit Service&lt;br&gt;Mammoth Hierarchy Class Listener&lt;br&gt;Mammoth Product Listener&lt;br&gt;Mammoth Item Locale Controller&lt;br&gt;Mammoth Web Support</t>
   </si>
   <si>
-    <t>03</t>
-  </si>
-  <si>
-    <t>160 - 164 (December 18 - February 28)</t>
-  </si>
-  <si>
-    <t>CHG0044494</t>
-  </si>
-  <si>
-    <t>RELEASE_2020_03</t>
-  </si>
-  <si>
-    <t>11.9</t>
-  </si>
-  <si>
-    <t>11.9.0</t>
-  </si>
-  <si>
     <t>Icon-DB-QA *AND* Icon-DB-QA-Perf</t>
   </si>
   <si>
-    <t>IrmaPriceListener,JobSchedulerService,PublishInventorySpoilageService,PublishPurchaseOrderService,PublishReceivedOrderService,PublishTransferOrderService,PublishKitsService</t>
-  </si>
-  <si>
-    <t>11.8.1</t>
-  </si>
-  <si>
     <t>&lt;ol&gt;&lt;li&gt;IRMA Web Service&lt;li&gt;IRMA Mobile Plugin DLL&lt;li&gt;WFM Mobile Config File&lt;/ol&gt;</t>
   </si>
   <si>
-    <t>IRMA Web Service, IRMA Mobile Plugin DLL, WFM Mobile Config File</t>
-  </si>
-  <si>
-    <t>&lt;hr&gt;IRMA Client&lt;br&gt;Icon DB&lt;br&gt;All Icon Apps&lt;br&gt;Mammoth DB&lt;br&gt;All Mammoth Apps</t>
-  </si>
-  <si>
     <t>IRMAQAJob[01-06], IRMAQAWeb[01-06]</t>
   </si>
   <si>
     <t>IRMAQAJob[01-06]</t>
+  </si>
+  <si>
+    <t>169 - 170 (April 22 - May 19)</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>12.1</t>
+  </si>
+  <si>
+    <t>12.1.0</t>
+  </si>
+  <si>
+    <t>IDQ-xx\xxQ</t>
+  </si>
+  <si>
+    <t>Icon-DB-QA</t>
+  </si>
+  <si>
+    <t>Mammoth-DB01-QA\Mammoth.Mammoth</t>
+  </si>
+  <si>
+    <t>IRMAQAWeb[01-06]</t>
+  </si>
+  <si>
+    <t>old: IRMAQAApp[1-4]</t>
+  </si>
+  <si>
+    <t>&lt;hr&gt;Icon DB&lt;br&gt;Mammoth DB&lt;br&gt;Icon API Controller&lt;br&gt;Icon Web&lt;br&gt;Icon Controller Monitor&lt;br&gt;Icon Item Publisher&lt;br&gt;Icon Bulk Item Upload&lt;br&gt;Icon Extract Service&lt;br&gt;Icon Brand Upload</t>
+  </si>
+  <si>
+    <t>CHG0046984</t>
+  </si>
+  <si>
+    <t>RELEASE_2020_06</t>
   </si>
 </sst>
 </file>
@@ -974,8 +974,8 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="A2:C63"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -989,13 +989,13 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1012,7 +1012,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>167</v>
+        <v>177</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1034,7 +1034,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1050,7 +1050,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>58</v>
@@ -1064,12 +1064,12 @@
         <v>8</v>
       </c>
       <c r="C7" s="6">
-        <v>43893</v>
+        <v>43977</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="8">
@@ -1078,20 +1078,20 @@
     </row>
     <row r="9" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1182,44 +1182,44 @@
     </row>
     <row r="21" spans="1:4" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
         <v>26</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D23" s="9"/>
     </row>
     <row r="24" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>87</v>
+      </c>
+      <c r="C24" s="9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" s="9" t="s">
         <v>88</v>
-      </c>
-      <c r="C24" s="9" t="s">
-        <v>121</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -1230,10 +1230,10 @@
         <v>11</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>168</v>
+        <v>178</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -1244,7 +1244,7 @@
         <v>47</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1266,7 +1266,7 @@
         <v>13</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1277,7 +1277,7 @@
         <v>48</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1370,7 +1370,10 @@
         <v>65</v>
       </c>
       <c r="C38" t="s">
-        <v>161</v>
+        <v>171</v>
+      </c>
+      <c r="D38" s="8" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -1378,7 +1381,10 @@
         <v>66</v>
       </c>
       <c r="C39" t="s">
-        <v>171</v>
+        <v>172</v>
+      </c>
+      <c r="D39" s="8" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -1408,74 +1414,77 @@
         <v>73</v>
       </c>
       <c r="C42" t="s">
-        <v>74</v>
+        <v>174</v>
+      </c>
+      <c r="D42" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B43" t="s">
         <v>73</v>
       </c>
       <c r="C43" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" t="s">
         <v>73</v>
       </c>
       <c r="C44" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" t="s">
         <v>73</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="180.75" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>172</v>
+        <v>138</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C48" s="8">
         <v>0</v>
@@ -1484,31 +1493,31 @@
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>61</v>
@@ -1516,48 +1525,51 @@
     </row>
     <row r="53" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>91</v>
+      </c>
+      <c r="B53" t="s">
         <v>92</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C53" s="9" t="s">
-        <v>174</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>94</v>
+      <c r="F53" t="s">
+        <v>164</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="F54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>108</v>
       </c>
-      <c r="C54" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="F54" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>109</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>175</v>
+      <c r="C55" s="9" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C56" s="1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C57" s="9" t="s">
         <v>176</v>
@@ -1565,56 +1577,56 @@
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B60" s="9" t="s">
-        <v>141</v>
-      </c>
       <c r="C60" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1644,13 +1656,13 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B1" s="9" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -1659,7 +1671,7 @@
         <v>1</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1670,7 +1682,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1692,7 +1704,7 @@
         <v>6</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1703,15 +1715,15 @@
         <v>7</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,7 +1739,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" s="8">
         <v>2020</v>
@@ -1735,20 +1747,20 @@
     </row>
     <row r="9" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="8" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1839,10 +1851,10 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D21" s="1"/>
     </row>
@@ -1854,7 +1866,7 @@
         <v>11</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -1865,7 +1877,7 @@
         <v>47</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -1896,7 +1908,7 @@
         <v>48</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -1916,7 +1928,7 @@
         <v>15</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -1924,7 +1936,7 @@
         <v>69</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -1976,43 +1988,43 @@
     </row>
     <row r="34" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B35" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D35" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E35" s="1" t="s">
-        <v>86</v>
-      </c>
       <c r="F35" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="36" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2028,7 +2040,7 @@
         <v>65</v>
       </c>
       <c r="C38" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -2036,7 +2048,7 @@
         <v>66</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -2044,7 +2056,7 @@
         <v>68</v>
       </c>
       <c r="C40" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -2066,74 +2078,74 @@
         <v>73</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B43" s="9" t="s">
         <v>73</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B44" s="9" t="s">
         <v>73</v>
       </c>
       <c r="C44" s="8" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B45" s="9" t="s">
         <v>73</v>
       </c>
       <c r="C45" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C46" s="9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="47" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B47" s="8" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C47" s="8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D47" s="11"/>
     </row>
     <row r="48" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C48" s="8">
         <v>0</v>
@@ -2142,34 +2154,34 @@
     </row>
     <row r="49" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C49" s="9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C50" s="8" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>89</v>
+      </c>
+      <c r="C51" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="C51" s="9" t="s">
-        <v>91</v>
-      </c>
       <c r="D51" s="9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>61</v>
@@ -2177,117 +2189,117 @@
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C53" s="9" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="54" spans="1:6" ht="120" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="9" t="s">
-        <v>93</v>
-      </c>
       <c r="C54" s="9" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D54" s="9"/>
       <c r="F54" s="9" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C55" s="9" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
+        <v>104</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>105</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="57" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C57" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D57" s="9" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F57" s="9"/>
     </row>
     <row r="58" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F58" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="59" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="60" spans="1:6" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B60" s="9" t="s">
-        <v>141</v>
-      </c>
       <c r="C60" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B62" s="9"/>
       <c r="C62" s="2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:6" s="8" customFormat="1" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B63" s="9"/>
       <c r="C63" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>